<commit_message>
src edit 8.26 11:35 update inst.xslx ex.v id.v
</commit_message>
<xml_diff>
--- a/指令.xlsx
+++ b/指令.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\cpu\bitmips_experiments-master\lab5\teach_soc\teach_soc.srcs\sources_1\new\myCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCB48FCA-D80F-4D44-A962-5E4CFBC4313E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310FE8FA-E43B-47DC-AFEB-9B831FB0CA2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="22365" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32760" yWindow="32760" windowWidth="22365" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="指令译码" sheetId="1" r:id="rId1"/>
+    <sheet name="id信号" sheetId="3" r:id="rId2"/>
+    <sheet name="alu信号" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="256">
   <si>
     <t>指令</t>
   </si>
@@ -2844,27 +2844,186 @@
     <t>转移指令</t>
   </si>
   <si>
+    <t>alu_op</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100000</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>101000</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>100001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>101001</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve">         alu信号
 指令</t>
-  </si>
-  <si>
-    <t>alu_op</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>100000</t>
+    <t xml:space="preserve">          id信号
+指令</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>101000</t>
+    <t>表示</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>100001</t>
+    <t>小可爱指令</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>101001</t>
+    <t>reg1_read_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_read_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_addr_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_addr_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aluop_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>alusel_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wd_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wreg_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>return_addr_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch_flag_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>branch_target_address_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc_o</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stallreq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>`ReadDisable
+`ReadEnable</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>信号候选值</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rs
+`ZeroRegAddr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt
+`ZeroRegAddr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg1_data_i
+imm16_signe
+imm16_unsigne
+`ZeroWord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>reg2_data_i
+imm16_signe
+imm16_unsigne
+imm26_signe
+imm26_unsigne
+`ZeroWord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>rt
+rd
+`ZeroRegAddr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>`WriteEnable
+`WriteDisable</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>待开发
+`ZeroRegAddr</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>`Branch
+`NotBranch</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>`InitialPc
+计算结果</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>inst_i
+`ZeroWord</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pc_i
+`InitialPc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>`Stop
+`NoStop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>有点多
+按指令写即可</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2872,7 +3031,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -2997,8 +3156,43 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3041,8 +3235,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -3140,13 +3346,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3234,6 +3464,90 @@
     <xf numFmtId="49" fontId="15" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="17" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="15" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3243,91 +3557,88 @@
     <xf numFmtId="49" fontId="15" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="17" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -3607,9 +3918,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D54" sqref="D54"/>
+      <selection pane="topRight" activeCell="L52" sqref="L52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
@@ -3637,11 +3948,11 @@
       <c r="I1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
     </row>
     <row r="2" spans="1:19" ht="54" x14ac:dyDescent="0.15">
       <c r="B2" s="6"/>
@@ -3669,14 +3980,14 @@
       <c r="J2" s="25"/>
       <c r="K2" s="4"/>
       <c r="L2" s="26"/>
-      <c r="M2" s="57"/>
-      <c r="N2" s="57"/>
-      <c r="O2" s="57"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="26"/>
       <c r="Q2" s="26"/>
       <c r="R2" s="26"/>
-      <c r="S2" s="60" t="s">
-        <v>217</v>
+      <c r="S2" s="30" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.15">
@@ -3708,11 +4019,11 @@
       </c>
       <c r="K3" s="37"/>
       <c r="L3" s="37"/>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
       <c r="P3" s="27"/>
       <c r="Q3" s="27"/>
       <c r="R3" s="27"/>
@@ -3749,15 +4060,15 @@
       </c>
       <c r="K4" s="37"/>
       <c r="L4" s="37"/>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
       <c r="P4" s="27"/>
       <c r="Q4" s="27"/>
       <c r="R4" s="27"/>
-      <c r="S4" s="60">
+      <c r="S4" s="30">
         <v>2</v>
       </c>
     </row>
@@ -3790,11 +4101,11 @@
       </c>
       <c r="K5" s="37"/>
       <c r="L5" s="37"/>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
       <c r="P5" s="27"/>
       <c r="Q5" s="27"/>
       <c r="R5" s="27"/>
@@ -3803,7 +4114,7 @@
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A6" s="2">
+      <c r="A6" s="64">
         <v>4</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -3835,15 +4146,15 @@
       </c>
       <c r="K6" s="37"/>
       <c r="L6" s="37"/>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
       <c r="P6" s="27"/>
       <c r="Q6" s="27"/>
       <c r="R6" s="27"/>
-      <c r="S6" s="60">
+      <c r="S6" s="30">
         <v>4</v>
       </c>
     </row>
@@ -3875,14 +4186,14 @@
       <c r="I7" s="12">
         <v>100111</v>
       </c>
-      <c r="J7" s="38"/>
-      <c r="K7" s="38"/>
-      <c r="L7" s="38"/>
-      <c r="M7" s="33" t="s">
+      <c r="J7" s="40"/>
+      <c r="K7" s="40"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
       <c r="P7" s="27"/>
       <c r="Q7" s="27"/>
       <c r="R7" s="27"/>
@@ -3923,15 +4234,15 @@
       </c>
       <c r="K8" s="37"/>
       <c r="L8" s="37"/>
-      <c r="M8" s="33" t="s">
+      <c r="M8" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
       <c r="P8" s="27"/>
       <c r="Q8" s="27"/>
       <c r="R8" s="27"/>
-      <c r="S8" s="60">
+      <c r="S8" s="30">
         <v>6</v>
       </c>
     </row>
@@ -3968,11 +4279,11 @@
       </c>
       <c r="K9" s="37"/>
       <c r="L9" s="37"/>
-      <c r="M9" s="33" t="s">
+      <c r="M9" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
       <c r="P9" s="27"/>
       <c r="Q9" s="27"/>
       <c r="R9" s="27"/>
@@ -4004,20 +4315,20 @@
       </c>
       <c r="H10" s="35"/>
       <c r="I10" s="36"/>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="K10" s="32"/>
-      <c r="L10" s="32"/>
-      <c r="M10" s="33" t="s">
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
       <c r="P10" s="27"/>
       <c r="Q10" s="27"/>
       <c r="R10" s="27"/>
-      <c r="S10" s="60">
+      <c r="S10" s="30">
         <v>8</v>
       </c>
     </row>
@@ -4049,16 +4360,16 @@
       <c r="I11" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J11" s="42" t="s">
+      <c r="J11" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="42"/>
-      <c r="L11" s="42"/>
-      <c r="M11" s="33" t="s">
+      <c r="K11" s="41"/>
+      <c r="L11" s="41"/>
+      <c r="M11" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="N11" s="33"/>
-      <c r="O11" s="33"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
       <c r="R11" s="27"/>
@@ -4094,20 +4405,20 @@
       <c r="I12" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="J12" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="33" t="s">
+      <c r="K12" s="42"/>
+      <c r="L12" s="42"/>
+      <c r="M12" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="N12" s="33"/>
-      <c r="O12" s="33"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
       <c r="P12" s="27"/>
       <c r="Q12" s="27"/>
       <c r="R12" s="27"/>
-      <c r="S12" s="60">
+      <c r="S12" s="30">
         <v>10</v>
       </c>
     </row>
@@ -4139,16 +4450,16 @@
       <c r="I13" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="32" t="s">
+      <c r="J13" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="41" t="s">
+      <c r="K13" s="39"/>
+      <c r="L13" s="39"/>
+      <c r="M13" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
+      <c r="N13" s="43"/>
+      <c r="O13" s="43"/>
       <c r="P13" s="27"/>
       <c r="Q13" s="27"/>
       <c r="R13" s="27"/>
@@ -4157,7 +4468,7 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A14" s="2">
+      <c r="A14" s="64">
         <v>12</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -4184,20 +4495,20 @@
       <c r="I14" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="J14" s="39" t="s">
+      <c r="J14" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="33" t="s">
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="N14" s="33"/>
-      <c r="O14" s="33"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
       <c r="P14" s="27"/>
       <c r="Q14" s="27"/>
       <c r="R14" s="27"/>
-      <c r="S14" s="60">
+      <c r="S14" s="30">
         <v>12</v>
       </c>
     </row>
@@ -4229,16 +4540,16 @@
       <c r="I15" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="J15" s="39" t="s">
+      <c r="J15" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="39"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="33" t="s">
+      <c r="K15" s="42"/>
+      <c r="L15" s="42"/>
+      <c r="M15" s="38" t="s">
         <v>80</v>
       </c>
-      <c r="N15" s="33"/>
-      <c r="O15" s="33"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="38"/>
       <c r="P15" s="27"/>
       <c r="Q15" s="27"/>
       <c r="R15" s="27"/>
@@ -4274,20 +4585,20 @@
       <c r="I16" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="J16" s="39" t="s">
+      <c r="J16" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="K16" s="39"/>
-      <c r="L16" s="39"/>
-      <c r="M16" s="33" t="s">
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="38" t="s">
         <v>85</v>
       </c>
-      <c r="N16" s="33"/>
-      <c r="O16" s="33"/>
+      <c r="N16" s="38"/>
+      <c r="O16" s="38"/>
       <c r="P16" s="27"/>
       <c r="Q16" s="27"/>
       <c r="R16" s="27"/>
-      <c r="S16" s="60">
+      <c r="S16" s="30">
         <v>14</v>
       </c>
     </row>
@@ -4319,14 +4630,14 @@
       <c r="I17" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J17" s="52" t="s">
+      <c r="J17" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="K17" s="53"/>
-      <c r="L17" s="54"/>
-      <c r="M17" s="46"/>
-      <c r="N17" s="47"/>
-      <c r="O17" s="48"/>
+      <c r="K17" s="45"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="47"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="49"/>
       <c r="P17" s="27"/>
       <c r="Q17" s="27"/>
       <c r="R17" s="27"/>
@@ -4362,18 +4673,18 @@
       <c r="I18" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="J18" s="52" t="s">
+      <c r="J18" s="44" t="s">
         <v>92</v>
       </c>
-      <c r="K18" s="53"/>
-      <c r="L18" s="54"/>
-      <c r="M18" s="46"/>
-      <c r="N18" s="47"/>
-      <c r="O18" s="48"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="49"/>
       <c r="P18" s="27"/>
       <c r="Q18" s="27"/>
       <c r="R18" s="27"/>
-      <c r="S18" s="60">
+      <c r="S18" s="30">
         <v>16</v>
       </c>
     </row>
@@ -4405,14 +4716,14 @@
       <c r="I19" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="J19" s="52" t="s">
+      <c r="J19" s="44" t="s">
         <v>95</v>
       </c>
-      <c r="K19" s="53"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="46"/>
-      <c r="N19" s="47"/>
-      <c r="O19" s="48"/>
+      <c r="K19" s="45"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="49"/>
       <c r="P19" s="27"/>
       <c r="Q19" s="27"/>
       <c r="R19" s="27"/>
@@ -4448,25 +4759,25 @@
       <c r="I20" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="J20" s="43"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="45"/>
-      <c r="M20" s="46" t="s">
+      <c r="J20" s="50"/>
+      <c r="K20" s="51"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="47" t="s">
         <v>99</v>
       </c>
-      <c r="N20" s="47"/>
-      <c r="O20" s="48"/>
-      <c r="P20" s="49" t="s">
+      <c r="N20" s="48"/>
+      <c r="O20" s="49"/>
+      <c r="P20" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="Q20" s="50"/>
-      <c r="R20" s="51"/>
-      <c r="S20" s="60">
+      <c r="Q20" s="54"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="30">
         <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A21" s="2">
+      <c r="A21" s="64">
         <v>19</v>
       </c>
       <c r="B21" s="14" t="s">
@@ -4493,14 +4804,14 @@
       <c r="I21" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="J21" s="43"/>
-      <c r="K21" s="44"/>
-      <c r="L21" s="45"/>
-      <c r="M21" s="46" t="s">
+      <c r="J21" s="50"/>
+      <c r="K21" s="51"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="47" t="s">
         <v>104</v>
       </c>
-      <c r="N21" s="47"/>
-      <c r="O21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="49"/>
       <c r="P21" s="27"/>
       <c r="Q21" s="27"/>
       <c r="R21" s="27"/>
@@ -4536,20 +4847,20 @@
       <c r="I22" s="28">
         <v>100000</v>
       </c>
-      <c r="J22" s="32" t="s">
+      <c r="J22" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-      <c r="M22" s="33" t="s">
+      <c r="K22" s="39"/>
+      <c r="L22" s="39"/>
+      <c r="M22" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
+      <c r="N22" s="38"/>
+      <c r="O22" s="38"/>
       <c r="P22" s="27"/>
       <c r="Q22" s="27"/>
       <c r="R22" s="27"/>
-      <c r="S22" s="60">
+      <c r="S22" s="30">
         <v>20</v>
       </c>
     </row>
@@ -4581,14 +4892,14 @@
       <c r="I23" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-      <c r="L23" s="38"/>
-      <c r="M23" s="33" t="s">
+      <c r="J23" s="40"/>
+      <c r="K23" s="40"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+      <c r="N23" s="38"/>
+      <c r="O23" s="38"/>
       <c r="P23" s="27"/>
       <c r="Q23" s="27"/>
       <c r="R23" s="27"/>
@@ -4629,15 +4940,15 @@
       </c>
       <c r="K24" s="37"/>
       <c r="L24" s="37"/>
-      <c r="M24" s="33" t="s">
+      <c r="M24" s="38" t="s">
         <v>116</v>
       </c>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
+      <c r="N24" s="38"/>
+      <c r="O24" s="38"/>
       <c r="P24" s="27"/>
       <c r="Q24" s="27"/>
       <c r="R24" s="27"/>
-      <c r="S24" s="60">
+      <c r="S24" s="30">
         <v>22</v>
       </c>
     </row>
@@ -4669,14 +4980,14 @@
       <c r="I25" s="12">
         <v>100011</v>
       </c>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="41" t="s">
+      <c r="J25" s="40"/>
+      <c r="K25" s="40"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
       <c r="P25" s="27"/>
       <c r="Q25" s="27"/>
       <c r="R25" s="27"/>
@@ -4712,18 +5023,18 @@
       <c r="I26" s="12">
         <v>101010</v>
       </c>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="33" t="s">
+      <c r="J26" s="40"/>
+      <c r="K26" s="40"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="38" t="s">
         <v>122</v>
       </c>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
-      <c r="P26" s="33"/>
-      <c r="Q26" s="33"/>
-      <c r="R26" s="33"/>
-      <c r="S26" s="60">
+      <c r="N26" s="38"/>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38"/>
+      <c r="R26" s="38"/>
+      <c r="S26" s="30">
         <v>24</v>
       </c>
     </row>
@@ -4755,17 +5066,17 @@
       <c r="I27" s="12">
         <v>101011</v>
       </c>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-      <c r="M27" s="33" t="s">
+      <c r="J27" s="40"/>
+      <c r="K27" s="40"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
+      <c r="N27" s="38"/>
+      <c r="O27" s="38"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
+      <c r="R27" s="38"/>
       <c r="S27">
         <v>25</v>
       </c>
@@ -4799,15 +5110,15 @@
       </c>
       <c r="K28" s="37"/>
       <c r="L28" s="37"/>
-      <c r="M28" s="33" t="s">
+      <c r="M28" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
-      <c r="P28" s="33"/>
-      <c r="Q28" s="33"/>
-      <c r="R28" s="33"/>
-      <c r="S28" s="60">
+      <c r="N28" s="38"/>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="S28" s="30">
         <v>26</v>
       </c>
     </row>
@@ -4835,25 +5146,25 @@
       </c>
       <c r="H29" s="35"/>
       <c r="I29" s="36"/>
-      <c r="J29" s="40" t="s">
+      <c r="J29" s="56" t="s">
         <v>134</v>
       </c>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="33" t="s">
+      <c r="K29" s="56"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="38" t="s">
         <v>135</v>
       </c>
-      <c r="N29" s="33"/>
-      <c r="O29" s="33"/>
-      <c r="P29" s="41"/>
-      <c r="Q29" s="41"/>
-      <c r="R29" s="41"/>
+      <c r="N29" s="38"/>
+      <c r="O29" s="38"/>
+      <c r="P29" s="43"/>
+      <c r="Q29" s="43"/>
+      <c r="R29" s="43"/>
       <c r="S29">
         <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A30" s="2">
+      <c r="A30" s="64">
         <v>28</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -4876,18 +5187,18 @@
       </c>
       <c r="H30" s="35"/>
       <c r="I30" s="36"/>
-      <c r="J30" s="38"/>
-      <c r="K30" s="38"/>
-      <c r="L30" s="38"/>
-      <c r="M30" s="33" t="s">
+      <c r="J30" s="40"/>
+      <c r="K30" s="40"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="38" t="s">
         <v>138</v>
       </c>
-      <c r="N30" s="33"/>
-      <c r="O30" s="33"/>
-      <c r="P30" s="33"/>
-      <c r="Q30" s="33"/>
-      <c r="R30" s="33"/>
-      <c r="S30" s="60">
+      <c r="N30" s="38"/>
+      <c r="O30" s="38"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="38"/>
+      <c r="S30" s="30">
         <v>28</v>
       </c>
     </row>
@@ -4915,17 +5226,17 @@
       </c>
       <c r="H31" s="35"/>
       <c r="I31" s="36"/>
-      <c r="J31" s="38"/>
-      <c r="K31" s="38"/>
-      <c r="L31" s="38"/>
-      <c r="M31" s="33" t="s">
+      <c r="J31" s="40"/>
+      <c r="K31" s="40"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
-      <c r="P31" s="33"/>
-      <c r="Q31" s="33"/>
-      <c r="R31" s="33"/>
+      <c r="N31" s="38"/>
+      <c r="O31" s="38"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="38"/>
       <c r="S31">
         <v>29</v>
       </c>
@@ -4943,27 +5254,27 @@
       <c r="D32" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="F32" s="30"/>
-      <c r="G32" s="30"/>
-      <c r="H32" s="30"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="32" t="s">
+      <c r="F32" s="58"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-      <c r="M32" s="33" t="s">
+      <c r="K32" s="39"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
-      <c r="P32" s="33"/>
-      <c r="Q32" s="33"/>
-      <c r="R32" s="33"/>
-      <c r="S32" s="60">
+      <c r="N32" s="38"/>
+      <c r="O32" s="38"/>
+      <c r="P32" s="38"/>
+      <c r="Q32" s="38"/>
+      <c r="R32" s="38"/>
+      <c r="S32" s="30">
         <v>30</v>
       </c>
     </row>
@@ -4980,24 +5291,24 @@
       <c r="D33" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="29" t="s">
+      <c r="E33" s="57" t="s">
         <v>144</v>
       </c>
-      <c r="F33" s="30"/>
-      <c r="G33" s="30"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="33" t="s">
+      <c r="F33" s="58"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="40"/>
+      <c r="K33" s="40"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
-      <c r="P33" s="33"/>
-      <c r="Q33" s="33"/>
-      <c r="R33" s="33"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
       <c r="S33">
         <v>31</v>
       </c>
@@ -5033,15 +5344,15 @@
       <c r="J34" s="37"/>
       <c r="K34" s="37"/>
       <c r="L34" s="37"/>
-      <c r="M34" s="33" t="s">
+      <c r="M34" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
-      <c r="P34" s="33"/>
-      <c r="Q34" s="33"/>
-      <c r="R34" s="33"/>
-      <c r="S34" s="60">
+      <c r="N34" s="38"/>
+      <c r="O34" s="38"/>
+      <c r="P34" s="38"/>
+      <c r="Q34" s="38"/>
+      <c r="R34" s="38"/>
+      <c r="S34" s="30">
         <v>32</v>
       </c>
     </row>
@@ -5073,17 +5384,17 @@
       <c r="I35" s="28" t="s">
         <v>133</v>
       </c>
-      <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-      <c r="M35" s="33" t="s">
+      <c r="J35" s="39"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="39"/>
+      <c r="M35" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
-      <c r="P35" s="33"/>
-      <c r="Q35" s="33"/>
-      <c r="R35" s="33"/>
+      <c r="N35" s="38"/>
+      <c r="O35" s="38"/>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
       <c r="S35">
         <v>33</v>
       </c>
@@ -5112,18 +5423,18 @@
       </c>
       <c r="H36" s="35"/>
       <c r="I36" s="36"/>
-      <c r="J36" s="38"/>
-      <c r="K36" s="38"/>
-      <c r="L36" s="38"/>
-      <c r="M36" s="33" t="s">
+      <c r="J36" s="40"/>
+      <c r="K36" s="40"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="N36" s="33"/>
-      <c r="O36" s="33"/>
-      <c r="P36" s="33"/>
-      <c r="Q36" s="33"/>
-      <c r="R36" s="33"/>
-      <c r="S36" s="60">
+      <c r="N36" s="38"/>
+      <c r="O36" s="38"/>
+      <c r="P36" s="38"/>
+      <c r="Q36" s="38"/>
+      <c r="R36" s="38"/>
+      <c r="S36" s="30">
         <v>34</v>
       </c>
     </row>
@@ -5154,20 +5465,20 @@
       <c r="J37" s="37"/>
       <c r="K37" s="37"/>
       <c r="L37" s="37"/>
-      <c r="M37" s="33" t="s">
+      <c r="M37" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="N37" s="33"/>
-      <c r="O37" s="33"/>
-      <c r="P37" s="33"/>
-      <c r="Q37" s="33"/>
-      <c r="R37" s="33"/>
+      <c r="N37" s="38"/>
+      <c r="O37" s="38"/>
+      <c r="P37" s="38"/>
+      <c r="Q37" s="38"/>
+      <c r="R37" s="38"/>
       <c r="S37">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A38" s="2">
+      <c r="A38" s="64">
         <v>36</v>
       </c>
       <c r="B38" s="10" t="s">
@@ -5190,18 +5501,18 @@
       </c>
       <c r="H38" s="35"/>
       <c r="I38" s="36"/>
-      <c r="J38" s="38"/>
-      <c r="K38" s="38"/>
-      <c r="L38" s="38"/>
-      <c r="M38" s="41" t="s">
+      <c r="J38" s="40"/>
+      <c r="K38" s="40"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="43" t="s">
         <v>165</v>
       </c>
-      <c r="N38" s="41"/>
-      <c r="O38" s="41"/>
-      <c r="P38" s="41"/>
-      <c r="Q38" s="41"/>
-      <c r="R38" s="41"/>
-      <c r="S38" s="60">
+      <c r="N38" s="43"/>
+      <c r="O38" s="43"/>
+      <c r="P38" s="43"/>
+      <c r="Q38" s="43"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="30">
         <v>36</v>
       </c>
     </row>
@@ -5229,17 +5540,17 @@
       </c>
       <c r="H39" s="35"/>
       <c r="I39" s="36"/>
-      <c r="J39" s="38"/>
-      <c r="K39" s="38"/>
-      <c r="L39" s="38"/>
-      <c r="M39" s="33" t="s">
+      <c r="J39" s="40"/>
+      <c r="K39" s="40"/>
+      <c r="L39" s="40"/>
+      <c r="M39" s="38" t="s">
         <v>168</v>
       </c>
-      <c r="N39" s="33"/>
-      <c r="O39" s="33"/>
-      <c r="P39" s="33"/>
-      <c r="Q39" s="33"/>
-      <c r="R39" s="33"/>
+      <c r="N39" s="38"/>
+      <c r="O39" s="38"/>
+      <c r="P39" s="38"/>
+      <c r="Q39" s="38"/>
+      <c r="R39" s="38"/>
       <c r="S39">
         <v>37</v>
       </c>
@@ -5268,18 +5579,18 @@
       </c>
       <c r="H40" s="35"/>
       <c r="I40" s="36"/>
-      <c r="J40" s="38"/>
-      <c r="K40" s="38"/>
-      <c r="L40" s="38"/>
-      <c r="M40" s="33" t="s">
+      <c r="J40" s="40"/>
+      <c r="K40" s="40"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="N40" s="33"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
-      <c r="R40" s="33"/>
-      <c r="S40" s="60">
+      <c r="N40" s="38"/>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38"/>
+      <c r="R40" s="38"/>
+      <c r="S40" s="30">
         <v>38</v>
       </c>
     </row>
@@ -5310,14 +5621,14 @@
       <c r="J41" s="37"/>
       <c r="K41" s="37"/>
       <c r="L41" s="37"/>
-      <c r="M41" s="33" t="s">
+      <c r="M41" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="N41" s="33"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
-      <c r="R41" s="33"/>
+      <c r="N41" s="38"/>
+      <c r="O41" s="38"/>
+      <c r="P41" s="38"/>
+      <c r="Q41" s="38"/>
+      <c r="R41" s="38"/>
       <c r="S41">
         <v>39</v>
       </c>
@@ -5346,18 +5657,18 @@
       </c>
       <c r="H42" s="35"/>
       <c r="I42" s="36"/>
-      <c r="J42" s="38"/>
-      <c r="K42" s="38"/>
-      <c r="L42" s="38"/>
-      <c r="M42" s="33" t="s">
+      <c r="J42" s="40"/>
+      <c r="K42" s="40"/>
+      <c r="L42" s="40"/>
+      <c r="M42" s="38" t="s">
         <v>180</v>
       </c>
-      <c r="N42" s="33"/>
-      <c r="O42" s="33"/>
-      <c r="P42" s="33"/>
-      <c r="Q42" s="33"/>
-      <c r="R42" s="33"/>
-      <c r="S42" s="60">
+      <c r="N42" s="38"/>
+      <c r="O42" s="38"/>
+      <c r="P42" s="38"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="38"/>
+      <c r="S42" s="30">
         <v>40</v>
       </c>
     </row>
@@ -5388,14 +5699,14 @@
       <c r="J43" s="37"/>
       <c r="K43" s="37"/>
       <c r="L43" s="37"/>
-      <c r="M43" s="33" t="s">
+      <c r="M43" s="38" t="s">
         <v>183</v>
       </c>
-      <c r="N43" s="33"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="33"/>
-      <c r="R43" s="33"/>
+      <c r="N43" s="38"/>
+      <c r="O43" s="38"/>
+      <c r="P43" s="38"/>
+      <c r="Q43" s="38"/>
+      <c r="R43" s="38"/>
       <c r="S43">
         <v>41</v>
       </c>
@@ -5427,15 +5738,15 @@
       <c r="J44" s="37"/>
       <c r="K44" s="37"/>
       <c r="L44" s="37"/>
-      <c r="M44" s="33" t="s">
+      <c r="M44" s="38" t="s">
         <v>187</v>
       </c>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
-      <c r="P44" s="33"/>
-      <c r="Q44" s="33"/>
-      <c r="R44" s="33"/>
-      <c r="S44" s="60">
+      <c r="N44" s="38"/>
+      <c r="O44" s="38"/>
+      <c r="P44" s="38"/>
+      <c r="Q44" s="38"/>
+      <c r="R44" s="38"/>
+      <c r="S44" s="30">
         <v>42</v>
       </c>
     </row>
@@ -5463,17 +5774,17 @@
       </c>
       <c r="H45" s="35"/>
       <c r="I45" s="36"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="42"/>
-      <c r="L45" s="42"/>
-      <c r="M45" s="33" t="s">
+      <c r="J45" s="41"/>
+      <c r="K45" s="41"/>
+      <c r="L45" s="41"/>
+      <c r="M45" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="N45" s="33"/>
-      <c r="O45" s="33"/>
-      <c r="P45" s="33"/>
-      <c r="Q45" s="33"/>
-      <c r="R45" s="33"/>
+      <c r="N45" s="38"/>
+      <c r="O45" s="38"/>
+      <c r="P45" s="38"/>
+      <c r="Q45" s="38"/>
+      <c r="R45" s="38"/>
       <c r="S45">
         <v>43</v>
       </c>
@@ -5502,20 +5813,20 @@
       </c>
       <c r="H46" s="35"/>
       <c r="I46" s="36"/>
-      <c r="J46" s="32" t="s">
+      <c r="J46" s="39" t="s">
         <v>193</v>
       </c>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="33" t="s">
+      <c r="K46" s="39"/>
+      <c r="L46" s="39"/>
+      <c r="M46" s="38" t="s">
         <v>194</v>
       </c>
-      <c r="N46" s="33"/>
-      <c r="O46" s="33"/>
-      <c r="P46" s="33"/>
-      <c r="Q46" s="33"/>
-      <c r="R46" s="33"/>
-      <c r="S46" s="60">
+      <c r="N46" s="38"/>
+      <c r="O46" s="38"/>
+      <c r="P46" s="38"/>
+      <c r="Q46" s="38"/>
+      <c r="R46" s="38"/>
+      <c r="S46" s="30">
         <v>44</v>
       </c>
     </row>
@@ -5543,19 +5854,19 @@
       </c>
       <c r="H47" s="35"/>
       <c r="I47" s="36"/>
-      <c r="J47" s="32" t="s">
+      <c r="J47" s="39" t="s">
         <v>197</v>
       </c>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-      <c r="M47" s="33" t="s">
+      <c r="K47" s="39"/>
+      <c r="L47" s="39"/>
+      <c r="M47" s="38" t="s">
         <v>198</v>
       </c>
-      <c r="N47" s="33"/>
-      <c r="O47" s="33"/>
-      <c r="P47" s="33"/>
-      <c r="Q47" s="33"/>
-      <c r="R47" s="33"/>
+      <c r="N47" s="38"/>
+      <c r="O47" s="38"/>
+      <c r="P47" s="38"/>
+      <c r="Q47" s="38"/>
+      <c r="R47" s="38"/>
       <c r="S47">
         <v>45</v>
       </c>
@@ -5571,7 +5882,7 @@
         <v>199</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E48" s="12" t="s">
         <v>18</v>
@@ -5584,20 +5895,20 @@
       </c>
       <c r="H48" s="35"/>
       <c r="I48" s="36"/>
-      <c r="J48" s="32" t="s">
+      <c r="J48" s="39" t="s">
         <v>200</v>
       </c>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="33" t="s">
+      <c r="K48" s="39"/>
+      <c r="L48" s="39"/>
+      <c r="M48" s="38" t="s">
         <v>201</v>
       </c>
-      <c r="N48" s="33"/>
-      <c r="O48" s="33"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="33"/>
-      <c r="R48" s="33"/>
-      <c r="S48" s="60">
+      <c r="N48" s="38"/>
+      <c r="O48" s="38"/>
+      <c r="P48" s="38"/>
+      <c r="Q48" s="38"/>
+      <c r="R48" s="38"/>
+      <c r="S48" s="30">
         <v>46</v>
       </c>
     </row>
@@ -5612,7 +5923,7 @@
         <v>202</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E49" s="12" t="s">
         <v>18</v>
@@ -5625,25 +5936,25 @@
       </c>
       <c r="H49" s="35"/>
       <c r="I49" s="36"/>
-      <c r="J49" s="32" t="s">
+      <c r="J49" s="39" t="s">
         <v>203</v>
       </c>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-      <c r="M49" s="33" t="s">
+      <c r="K49" s="39"/>
+      <c r="L49" s="39"/>
+      <c r="M49" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="N49" s="33"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
-      <c r="R49" s="33"/>
+      <c r="N49" s="38"/>
+      <c r="O49" s="38"/>
+      <c r="P49" s="38"/>
+      <c r="Q49" s="38"/>
+      <c r="R49" s="38"/>
       <c r="S49">
         <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A50" s="2">
+      <c r="A50" s="64">
         <v>48</v>
       </c>
       <c r="B50" s="20" t="s">
@@ -5653,7 +5964,7 @@
         <v>205</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E50" s="12" t="s">
         <v>18</v>
@@ -5666,20 +5977,20 @@
       </c>
       <c r="H50" s="35"/>
       <c r="I50" s="36"/>
-      <c r="J50" s="32" t="s">
+      <c r="J50" s="39" t="s">
         <v>206</v>
       </c>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-      <c r="M50" s="33" t="s">
+      <c r="K50" s="39"/>
+      <c r="L50" s="39"/>
+      <c r="M50" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="N50" s="33"/>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="33"/>
-      <c r="S50" s="60">
+      <c r="N50" s="38"/>
+      <c r="O50" s="38"/>
+      <c r="P50" s="38"/>
+      <c r="Q50" s="38"/>
+      <c r="R50" s="38"/>
+      <c r="S50" s="30">
         <v>48</v>
       </c>
     </row>
@@ -5694,7 +6005,7 @@
         <v>208</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E51" s="12" t="s">
         <v>18</v>
@@ -5707,57 +6018,57 @@
       </c>
       <c r="H51" s="35"/>
       <c r="I51" s="36"/>
-      <c r="J51" s="32" t="s">
+      <c r="J51" s="39" t="s">
         <v>209</v>
       </c>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-      <c r="M51" s="33" t="s">
+      <c r="K51" s="39"/>
+      <c r="L51" s="39"/>
+      <c r="M51" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="N51" s="33"/>
-      <c r="O51" s="33"/>
-      <c r="P51" s="33"/>
-      <c r="Q51" s="33"/>
-      <c r="R51" s="33"/>
+      <c r="N51" s="38"/>
+      <c r="O51" s="38"/>
+      <c r="P51" s="38"/>
+      <c r="Q51" s="38"/>
+      <c r="R51" s="38"/>
       <c r="S51">
         <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P52" s="33"/>
-      <c r="Q52" s="33"/>
-      <c r="R52" s="33"/>
+      <c r="P52" s="38"/>
+      <c r="Q52" s="38"/>
+      <c r="R52" s="38"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P53" s="33"/>
-      <c r="Q53" s="33"/>
-      <c r="R53" s="33"/>
+      <c r="P53" s="38"/>
+      <c r="Q53" s="38"/>
+      <c r="R53" s="38"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P54" s="33"/>
-      <c r="Q54" s="33"/>
-      <c r="R54" s="33"/>
+      <c r="P54" s="38"/>
+      <c r="Q54" s="38"/>
+      <c r="R54" s="38"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P55" s="33"/>
-      <c r="Q55" s="33"/>
-      <c r="R55" s="33"/>
+      <c r="P55" s="38"/>
+      <c r="Q55" s="38"/>
+      <c r="R55" s="38"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P56" s="33"/>
-      <c r="Q56" s="33"/>
-      <c r="R56" s="33"/>
+      <c r="P56" s="38"/>
+      <c r="Q56" s="38"/>
+      <c r="R56" s="38"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P57" s="33"/>
-      <c r="Q57" s="33"/>
-      <c r="R57" s="33"/>
+      <c r="P57" s="38"/>
+      <c r="Q57" s="38"/>
+      <c r="R57" s="38"/>
     </row>
     <row r="58" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="P58" s="33"/>
-      <c r="Q58" s="33"/>
-      <c r="R58" s="33"/>
+      <c r="P58" s="38"/>
+      <c r="Q58" s="38"/>
+      <c r="R58" s="38"/>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.15">
       <c r="A59" t="s">
@@ -5787,6 +6098,15 @@
       </c>
       <c r="D61" t="s">
         <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.15">
+      <c r="B62" s="63"/>
+      <c r="C62" s="30" t="s">
+        <v>223</v>
+      </c>
+      <c r="D62" s="30" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="79" spans="2:15" x14ac:dyDescent="0.15">
@@ -5798,12 +6118,12 @@
       <c r="G79" s="12"/>
       <c r="H79" s="12"/>
       <c r="I79" s="28"/>
-      <c r="J79" s="32"/>
-      <c r="K79" s="32"/>
-      <c r="L79" s="32"/>
-      <c r="M79" s="33"/>
-      <c r="N79" s="33"/>
-      <c r="O79" s="33"/>
+      <c r="J79" s="39"/>
+      <c r="K79" s="39"/>
+      <c r="L79" s="39"/>
+      <c r="M79" s="38"/>
+      <c r="N79" s="38"/>
+      <c r="O79" s="38"/>
     </row>
     <row r="80" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B80" s="10"/>
@@ -5814,12 +6134,12 @@
       <c r="G80" s="12"/>
       <c r="H80" s="12"/>
       <c r="I80" s="28"/>
-      <c r="J80" s="38"/>
-      <c r="K80" s="38"/>
-      <c r="L80" s="38"/>
-      <c r="M80" s="33"/>
-      <c r="N80" s="33"/>
-      <c r="O80" s="33"/>
+      <c r="J80" s="40"/>
+      <c r="K80" s="40"/>
+      <c r="L80" s="40"/>
+      <c r="M80" s="38"/>
+      <c r="N80" s="38"/>
+      <c r="O80" s="38"/>
     </row>
     <row r="81" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B81" s="10"/>
@@ -5833,9 +6153,9 @@
       <c r="J81" s="37"/>
       <c r="K81" s="37"/>
       <c r="L81" s="37"/>
-      <c r="M81" s="33"/>
-      <c r="N81" s="33"/>
-      <c r="O81" s="33"/>
+      <c r="M81" s="38"/>
+      <c r="N81" s="38"/>
+      <c r="O81" s="38"/>
     </row>
     <row r="82" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B82" s="10"/>
@@ -5846,12 +6166,12 @@
       <c r="G82" s="12"/>
       <c r="H82" s="12"/>
       <c r="I82" s="12"/>
-      <c r="J82" s="38"/>
-      <c r="K82" s="38"/>
-      <c r="L82" s="38"/>
-      <c r="M82" s="41"/>
-      <c r="N82" s="41"/>
-      <c r="O82" s="41"/>
+      <c r="J82" s="40"/>
+      <c r="K82" s="40"/>
+      <c r="L82" s="40"/>
+      <c r="M82" s="43"/>
+      <c r="N82" s="43"/>
+      <c r="O82" s="43"/>
     </row>
     <row r="83" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B83" s="10"/>
@@ -5862,12 +6182,12 @@
       <c r="G83" s="12"/>
       <c r="H83" s="12"/>
       <c r="I83" s="12"/>
-      <c r="J83" s="38"/>
-      <c r="K83" s="38"/>
-      <c r="L83" s="38"/>
-      <c r="M83" s="33"/>
-      <c r="N83" s="33"/>
-      <c r="O83" s="33"/>
+      <c r="J83" s="40"/>
+      <c r="K83" s="40"/>
+      <c r="L83" s="40"/>
+      <c r="M83" s="38"/>
+      <c r="N83" s="38"/>
+      <c r="O83" s="38"/>
     </row>
     <row r="84" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B84" s="10"/>
@@ -5878,12 +6198,12 @@
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
       <c r="I84" s="12"/>
-      <c r="J84" s="38"/>
-      <c r="K84" s="38"/>
-      <c r="L84" s="38"/>
-      <c r="M84" s="33"/>
-      <c r="N84" s="33"/>
-      <c r="O84" s="33"/>
+      <c r="J84" s="40"/>
+      <c r="K84" s="40"/>
+      <c r="L84" s="40"/>
+      <c r="M84" s="38"/>
+      <c r="N84" s="38"/>
+      <c r="O84" s="38"/>
     </row>
     <row r="85" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B85" s="10"/>
@@ -5897,9 +6217,9 @@
       <c r="J85" s="37"/>
       <c r="K85" s="37"/>
       <c r="L85" s="37"/>
-      <c r="M85" s="33"/>
-      <c r="N85" s="33"/>
-      <c r="O85" s="33"/>
+      <c r="M85" s="38"/>
+      <c r="N85" s="38"/>
+      <c r="O85" s="38"/>
     </row>
     <row r="86" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B86" s="10"/>
@@ -5910,12 +6230,12 @@
       <c r="G86" s="12"/>
       <c r="H86" s="12"/>
       <c r="I86" s="12"/>
-      <c r="J86" s="38"/>
-      <c r="K86" s="38"/>
-      <c r="L86" s="38"/>
-      <c r="M86" s="33"/>
-      <c r="N86" s="33"/>
-      <c r="O86" s="33"/>
+      <c r="J86" s="40"/>
+      <c r="K86" s="40"/>
+      <c r="L86" s="40"/>
+      <c r="M86" s="38"/>
+      <c r="N86" s="38"/>
+      <c r="O86" s="38"/>
     </row>
     <row r="87" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B87" s="10"/>
@@ -5929,9 +6249,9 @@
       <c r="J87" s="37"/>
       <c r="K87" s="37"/>
       <c r="L87" s="37"/>
-      <c r="M87" s="33"/>
-      <c r="N87" s="33"/>
-      <c r="O87" s="33"/>
+      <c r="M87" s="38"/>
+      <c r="N87" s="38"/>
+      <c r="O87" s="38"/>
     </row>
     <row r="88" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B88" s="10"/>
@@ -5945,9 +6265,9 @@
       <c r="J88" s="37"/>
       <c r="K88" s="37"/>
       <c r="L88" s="37"/>
-      <c r="M88" s="33"/>
-      <c r="N88" s="33"/>
-      <c r="O88" s="33"/>
+      <c r="M88" s="38"/>
+      <c r="N88" s="38"/>
+      <c r="O88" s="38"/>
     </row>
     <row r="89" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B89" s="10"/>
@@ -5958,12 +6278,12 @@
       <c r="G89" s="12"/>
       <c r="H89" s="12"/>
       <c r="I89" s="12"/>
-      <c r="J89" s="42"/>
-      <c r="K89" s="42"/>
-      <c r="L89" s="42"/>
-      <c r="M89" s="33"/>
-      <c r="N89" s="33"/>
-      <c r="O89" s="33"/>
+      <c r="J89" s="41"/>
+      <c r="K89" s="41"/>
+      <c r="L89" s="41"/>
+      <c r="M89" s="38"/>
+      <c r="N89" s="38"/>
+      <c r="O89" s="38"/>
     </row>
     <row r="90" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B90" s="10"/>
@@ -5974,12 +6294,12 @@
       <c r="G90" s="12"/>
       <c r="H90" s="12"/>
       <c r="I90" s="12"/>
-      <c r="J90" s="39"/>
-      <c r="K90" s="39"/>
-      <c r="L90" s="39"/>
-      <c r="M90" s="33"/>
-      <c r="N90" s="33"/>
-      <c r="O90" s="33"/>
+      <c r="J90" s="42"/>
+      <c r="K90" s="42"/>
+      <c r="L90" s="42"/>
+      <c r="M90" s="38"/>
+      <c r="N90" s="38"/>
+      <c r="O90" s="38"/>
     </row>
     <row r="91" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B91" s="10"/>
@@ -5990,12 +6310,12 @@
       <c r="G91" s="12"/>
       <c r="H91" s="12"/>
       <c r="I91" s="12"/>
-      <c r="J91" s="32"/>
-      <c r="K91" s="32"/>
-      <c r="L91" s="32"/>
-      <c r="M91" s="41"/>
-      <c r="N91" s="41"/>
-      <c r="O91" s="41"/>
+      <c r="J91" s="39"/>
+      <c r="K91" s="39"/>
+      <c r="L91" s="39"/>
+      <c r="M91" s="43"/>
+      <c r="N91" s="43"/>
+      <c r="O91" s="43"/>
     </row>
     <row r="92" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B92" s="10"/>
@@ -6006,12 +6326,12 @@
       <c r="G92" s="12"/>
       <c r="H92" s="12"/>
       <c r="I92" s="12"/>
-      <c r="J92" s="39"/>
-      <c r="K92" s="39"/>
-      <c r="L92" s="39"/>
-      <c r="M92" s="33"/>
-      <c r="N92" s="33"/>
-      <c r="O92" s="33"/>
+      <c r="J92" s="42"/>
+      <c r="K92" s="42"/>
+      <c r="L92" s="42"/>
+      <c r="M92" s="38"/>
+      <c r="N92" s="38"/>
+      <c r="O92" s="38"/>
     </row>
     <row r="93" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B93" s="10"/>
@@ -6022,12 +6342,12 @@
       <c r="G93" s="12"/>
       <c r="H93" s="12"/>
       <c r="I93" s="12"/>
-      <c r="J93" s="39"/>
-      <c r="K93" s="39"/>
-      <c r="L93" s="39"/>
-      <c r="M93" s="33"/>
-      <c r="N93" s="33"/>
-      <c r="O93" s="33"/>
+      <c r="J93" s="42"/>
+      <c r="K93" s="42"/>
+      <c r="L93" s="42"/>
+      <c r="M93" s="38"/>
+      <c r="N93" s="38"/>
+      <c r="O93" s="38"/>
     </row>
     <row r="94" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B94" s="10"/>
@@ -6038,12 +6358,12 @@
       <c r="G94" s="12"/>
       <c r="H94" s="12"/>
       <c r="I94" s="12"/>
-      <c r="J94" s="39"/>
-      <c r="K94" s="39"/>
-      <c r="L94" s="39"/>
-      <c r="M94" s="33"/>
-      <c r="N94" s="33"/>
-      <c r="O94" s="33"/>
+      <c r="J94" s="42"/>
+      <c r="K94" s="42"/>
+      <c r="L94" s="42"/>
+      <c r="M94" s="38"/>
+      <c r="N94" s="38"/>
+      <c r="O94" s="38"/>
     </row>
     <row r="95" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B95" s="10"/>
@@ -6057,9 +6377,9 @@
       <c r="J95" s="37"/>
       <c r="K95" s="37"/>
       <c r="L95" s="37"/>
-      <c r="M95" s="33"/>
-      <c r="N95" s="33"/>
-      <c r="O95" s="33"/>
+      <c r="M95" s="38"/>
+      <c r="N95" s="38"/>
+      <c r="O95" s="38"/>
     </row>
     <row r="96" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B96" s="10"/>
@@ -6070,12 +6390,12 @@
       <c r="G96" s="34"/>
       <c r="H96" s="35"/>
       <c r="I96" s="36"/>
-      <c r="J96" s="40"/>
-      <c r="K96" s="40"/>
-      <c r="L96" s="40"/>
-      <c r="M96" s="33"/>
-      <c r="N96" s="33"/>
-      <c r="O96" s="33"/>
+      <c r="J96" s="56"/>
+      <c r="K96" s="56"/>
+      <c r="L96" s="56"/>
+      <c r="M96" s="38"/>
+      <c r="N96" s="38"/>
+      <c r="O96" s="38"/>
     </row>
     <row r="97" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B97" s="10"/>
@@ -6086,12 +6406,12 @@
       <c r="G97" s="34"/>
       <c r="H97" s="35"/>
       <c r="I97" s="36"/>
-      <c r="J97" s="38"/>
-      <c r="K97" s="38"/>
-      <c r="L97" s="38"/>
-      <c r="M97" s="33"/>
-      <c r="N97" s="33"/>
-      <c r="O97" s="33"/>
+      <c r="J97" s="40"/>
+      <c r="K97" s="40"/>
+      <c r="L97" s="40"/>
+      <c r="M97" s="38"/>
+      <c r="N97" s="38"/>
+      <c r="O97" s="38"/>
     </row>
     <row r="98" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B98" s="10"/>
@@ -6102,12 +6422,12 @@
       <c r="G98" s="34"/>
       <c r="H98" s="35"/>
       <c r="I98" s="36"/>
-      <c r="J98" s="38"/>
-      <c r="K98" s="38"/>
-      <c r="L98" s="38"/>
-      <c r="M98" s="33"/>
-      <c r="N98" s="33"/>
-      <c r="O98" s="33"/>
+      <c r="J98" s="40"/>
+      <c r="K98" s="40"/>
+      <c r="L98" s="40"/>
+      <c r="M98" s="38"/>
+      <c r="N98" s="38"/>
+      <c r="O98" s="38"/>
     </row>
     <row r="99" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B99" s="10"/>
@@ -6121,9 +6441,9 @@
       <c r="J99" s="37"/>
       <c r="K99" s="37"/>
       <c r="L99" s="37"/>
-      <c r="M99" s="33"/>
-      <c r="N99" s="33"/>
-      <c r="O99" s="33"/>
+      <c r="M99" s="38"/>
+      <c r="N99" s="38"/>
+      <c r="O99" s="38"/>
     </row>
     <row r="100" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B100" s="10"/>
@@ -6137,9 +6457,9 @@
       <c r="J100" s="37"/>
       <c r="K100" s="37"/>
       <c r="L100" s="37"/>
-      <c r="M100" s="33"/>
-      <c r="N100" s="33"/>
-      <c r="O100" s="33"/>
+      <c r="M100" s="38"/>
+      <c r="N100" s="38"/>
+      <c r="O100" s="38"/>
     </row>
     <row r="101" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B101" s="10"/>
@@ -6153,9 +6473,9 @@
       <c r="J101" s="37"/>
       <c r="K101" s="37"/>
       <c r="L101" s="37"/>
-      <c r="M101" s="33"/>
-      <c r="N101" s="33"/>
-      <c r="O101" s="33"/>
+      <c r="M101" s="38"/>
+      <c r="N101" s="38"/>
+      <c r="O101" s="38"/>
     </row>
     <row r="102" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B102" s="10"/>
@@ -6166,12 +6486,12 @@
       <c r="G102" s="34"/>
       <c r="H102" s="35"/>
       <c r="I102" s="36"/>
-      <c r="J102" s="32"/>
-      <c r="K102" s="32"/>
-      <c r="L102" s="32"/>
-      <c r="M102" s="33"/>
-      <c r="N102" s="33"/>
-      <c r="O102" s="33"/>
+      <c r="J102" s="39"/>
+      <c r="K102" s="39"/>
+      <c r="L102" s="39"/>
+      <c r="M102" s="38"/>
+      <c r="N102" s="38"/>
+      <c r="O102" s="38"/>
     </row>
     <row r="103" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B103" s="10"/>
@@ -6182,12 +6502,12 @@
       <c r="G103" s="34"/>
       <c r="H103" s="35"/>
       <c r="I103" s="36"/>
-      <c r="J103" s="32"/>
-      <c r="K103" s="32"/>
-      <c r="L103" s="32"/>
-      <c r="M103" s="33"/>
-      <c r="N103" s="33"/>
-      <c r="O103" s="33"/>
+      <c r="J103" s="39"/>
+      <c r="K103" s="39"/>
+      <c r="L103" s="39"/>
+      <c r="M103" s="38"/>
+      <c r="N103" s="38"/>
+      <c r="O103" s="38"/>
     </row>
     <row r="104" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B104" s="10"/>
@@ -6201,9 +6521,9 @@
       <c r="J104" s="37"/>
       <c r="K104" s="37"/>
       <c r="L104" s="37"/>
-      <c r="M104" s="33"/>
-      <c r="N104" s="33"/>
-      <c r="O104" s="33"/>
+      <c r="M104" s="38"/>
+      <c r="N104" s="38"/>
+      <c r="O104" s="38"/>
     </row>
     <row r="105" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B105" s="10"/>
@@ -6214,12 +6534,12 @@
       <c r="G105" s="34"/>
       <c r="H105" s="35"/>
       <c r="I105" s="36"/>
-      <c r="J105" s="32"/>
-      <c r="K105" s="32"/>
-      <c r="L105" s="32"/>
-      <c r="M105" s="33"/>
-      <c r="N105" s="33"/>
-      <c r="O105" s="33"/>
+      <c r="J105" s="39"/>
+      <c r="K105" s="39"/>
+      <c r="L105" s="39"/>
+      <c r="M105" s="38"/>
+      <c r="N105" s="38"/>
+      <c r="O105" s="38"/>
     </row>
     <row r="106" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B106" s="10"/>
@@ -6230,12 +6550,12 @@
       <c r="G106" s="34"/>
       <c r="H106" s="35"/>
       <c r="I106" s="36"/>
-      <c r="J106" s="32"/>
-      <c r="K106" s="32"/>
-      <c r="L106" s="32"/>
-      <c r="M106" s="33"/>
-      <c r="N106" s="33"/>
-      <c r="O106" s="33"/>
+      <c r="J106" s="39"/>
+      <c r="K106" s="39"/>
+      <c r="L106" s="39"/>
+      <c r="M106" s="38"/>
+      <c r="N106" s="38"/>
+      <c r="O106" s="38"/>
     </row>
     <row r="107" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B107" s="20"/>
@@ -6246,12 +6566,12 @@
       <c r="G107" s="34"/>
       <c r="H107" s="35"/>
       <c r="I107" s="36"/>
-      <c r="J107" s="32"/>
-      <c r="K107" s="32"/>
-      <c r="L107" s="32"/>
-      <c r="M107" s="33"/>
-      <c r="N107" s="33"/>
-      <c r="O107" s="33"/>
+      <c r="J107" s="39"/>
+      <c r="K107" s="39"/>
+      <c r="L107" s="39"/>
+      <c r="M107" s="38"/>
+      <c r="N107" s="38"/>
+      <c r="O107" s="38"/>
     </row>
     <row r="108" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B108" s="20"/>
@@ -6262,12 +6582,12 @@
       <c r="G108" s="34"/>
       <c r="H108" s="35"/>
       <c r="I108" s="36"/>
-      <c r="J108" s="32"/>
-      <c r="K108" s="32"/>
-      <c r="L108" s="32"/>
-      <c r="M108" s="33"/>
-      <c r="N108" s="33"/>
-      <c r="O108" s="33"/>
+      <c r="J108" s="39"/>
+      <c r="K108" s="39"/>
+      <c r="L108" s="39"/>
+      <c r="M108" s="38"/>
+      <c r="N108" s="38"/>
+      <c r="O108" s="38"/>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B109" s="20"/>
@@ -6278,12 +6598,12 @@
       <c r="G109" s="34"/>
       <c r="H109" s="35"/>
       <c r="I109" s="36"/>
-      <c r="J109" s="32"/>
-      <c r="K109" s="32"/>
-      <c r="L109" s="32"/>
-      <c r="M109" s="33"/>
-      <c r="N109" s="33"/>
-      <c r="O109" s="33"/>
+      <c r="J109" s="39"/>
+      <c r="K109" s="39"/>
+      <c r="L109" s="39"/>
+      <c r="M109" s="38"/>
+      <c r="N109" s="38"/>
+      <c r="O109" s="38"/>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B110" s="20"/>
@@ -6294,31 +6614,256 @@
       <c r="G110" s="34"/>
       <c r="H110" s="35"/>
       <c r="I110" s="36"/>
-      <c r="J110" s="32"/>
-      <c r="K110" s="32"/>
-      <c r="L110" s="32"/>
-      <c r="M110" s="33"/>
-      <c r="N110" s="33"/>
-      <c r="O110" s="33"/>
+      <c r="J110" s="39"/>
+      <c r="K110" s="39"/>
+      <c r="L110" s="39"/>
+      <c r="M110" s="38"/>
+      <c r="N110" s="38"/>
+      <c r="O110" s="38"/>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.15">
       <c r="B111" s="10"/>
       <c r="C111" s="17"/>
       <c r="D111" s="12"/>
-      <c r="E111" s="29"/>
-      <c r="F111" s="30"/>
-      <c r="G111" s="30"/>
-      <c r="H111" s="30"/>
-      <c r="I111" s="31"/>
-      <c r="J111" s="32"/>
-      <c r="K111" s="32"/>
-      <c r="L111" s="32"/>
-      <c r="M111" s="33"/>
-      <c r="N111" s="33"/>
-      <c r="O111" s="33"/>
+      <c r="E111" s="57"/>
+      <c r="F111" s="58"/>
+      <c r="G111" s="58"/>
+      <c r="H111" s="58"/>
+      <c r="I111" s="59"/>
+      <c r="J111" s="39"/>
+      <c r="K111" s="39"/>
+      <c r="L111" s="39"/>
+      <c r="M111" s="38"/>
+      <c r="N111" s="38"/>
+      <c r="O111" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="243">
+    <mergeCell ref="E111:I111"/>
+    <mergeCell ref="J111:L111"/>
+    <mergeCell ref="M111:O111"/>
+    <mergeCell ref="G109:I109"/>
+    <mergeCell ref="J109:L109"/>
+    <mergeCell ref="M109:O109"/>
+    <mergeCell ref="G110:I110"/>
+    <mergeCell ref="J110:L110"/>
+    <mergeCell ref="M110:O110"/>
+    <mergeCell ref="G107:I107"/>
+    <mergeCell ref="J107:L107"/>
+    <mergeCell ref="M107:O107"/>
+    <mergeCell ref="G108:I108"/>
+    <mergeCell ref="J108:L108"/>
+    <mergeCell ref="M108:O108"/>
+    <mergeCell ref="G105:I105"/>
+    <mergeCell ref="J105:L105"/>
+    <mergeCell ref="M105:O105"/>
+    <mergeCell ref="G106:I106"/>
+    <mergeCell ref="J106:L106"/>
+    <mergeCell ref="M106:O106"/>
+    <mergeCell ref="G103:I103"/>
+    <mergeCell ref="J103:L103"/>
+    <mergeCell ref="M103:O103"/>
+    <mergeCell ref="G104:I104"/>
+    <mergeCell ref="J104:L104"/>
+    <mergeCell ref="M104:O104"/>
+    <mergeCell ref="G101:I101"/>
+    <mergeCell ref="J101:L101"/>
+    <mergeCell ref="M101:O101"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="J102:L102"/>
+    <mergeCell ref="M102:O102"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="J99:L99"/>
+    <mergeCell ref="M99:O99"/>
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="J100:L100"/>
+    <mergeCell ref="M100:O100"/>
+    <mergeCell ref="G97:I97"/>
+    <mergeCell ref="J97:L97"/>
+    <mergeCell ref="M97:O97"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="J98:L98"/>
+    <mergeCell ref="M98:O98"/>
+    <mergeCell ref="J94:L94"/>
+    <mergeCell ref="M94:O94"/>
+    <mergeCell ref="G95:I95"/>
+    <mergeCell ref="J95:L95"/>
+    <mergeCell ref="M95:O95"/>
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="J96:L96"/>
+    <mergeCell ref="M96:O96"/>
+    <mergeCell ref="J91:L91"/>
+    <mergeCell ref="M91:O91"/>
+    <mergeCell ref="J92:L92"/>
+    <mergeCell ref="M92:O92"/>
+    <mergeCell ref="J93:L93"/>
+    <mergeCell ref="M93:O93"/>
+    <mergeCell ref="J88:L88"/>
+    <mergeCell ref="M88:O88"/>
+    <mergeCell ref="J89:L89"/>
+    <mergeCell ref="M89:O89"/>
+    <mergeCell ref="J90:L90"/>
+    <mergeCell ref="M90:O90"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:O85"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M86:O86"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M87:O87"/>
+    <mergeCell ref="J82:L82"/>
+    <mergeCell ref="M82:O82"/>
+    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="M83:O83"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:O84"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="J79:L79"/>
+    <mergeCell ref="M79:O79"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="M80:O80"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="M81:O81"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="P53:R53"/>
+    <mergeCell ref="P54:R54"/>
+    <mergeCell ref="P55:R55"/>
+    <mergeCell ref="P56:R56"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="P50:R50"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="P49:R49"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="P46:R46"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="P47:R47"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="P43:R43"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="P40:R40"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="G3:I3"/>
@@ -6337,231 +6882,6 @@
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:O7"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="P36:R36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="P39:R39"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="P43:R43"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="P49:R49"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="P46:R46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="P47:R47"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="P53:R53"/>
-    <mergeCell ref="P54:R54"/>
-    <mergeCell ref="P55:R55"/>
-    <mergeCell ref="P56:R56"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="P50:R50"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="J82:L82"/>
-    <mergeCell ref="M82:O82"/>
-    <mergeCell ref="J83:L83"/>
-    <mergeCell ref="M83:O83"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:O84"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="J79:L79"/>
-    <mergeCell ref="M79:O79"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="M80:O80"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="M81:O81"/>
-    <mergeCell ref="J88:L88"/>
-    <mergeCell ref="M88:O88"/>
-    <mergeCell ref="J89:L89"/>
-    <mergeCell ref="M89:O89"/>
-    <mergeCell ref="J90:L90"/>
-    <mergeCell ref="M90:O90"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:O85"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M86:O86"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M87:O87"/>
-    <mergeCell ref="J94:L94"/>
-    <mergeCell ref="M94:O94"/>
-    <mergeCell ref="G95:I95"/>
-    <mergeCell ref="J95:L95"/>
-    <mergeCell ref="M95:O95"/>
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="J96:L96"/>
-    <mergeCell ref="M96:O96"/>
-    <mergeCell ref="J91:L91"/>
-    <mergeCell ref="M91:O91"/>
-    <mergeCell ref="J92:L92"/>
-    <mergeCell ref="M92:O92"/>
-    <mergeCell ref="J93:L93"/>
-    <mergeCell ref="M93:O93"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="J99:L99"/>
-    <mergeCell ref="M99:O99"/>
-    <mergeCell ref="G100:I100"/>
-    <mergeCell ref="J100:L100"/>
-    <mergeCell ref="M100:O100"/>
-    <mergeCell ref="G97:I97"/>
-    <mergeCell ref="J97:L97"/>
-    <mergeCell ref="M97:O97"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="J98:L98"/>
-    <mergeCell ref="M98:O98"/>
-    <mergeCell ref="G103:I103"/>
-    <mergeCell ref="J103:L103"/>
-    <mergeCell ref="M103:O103"/>
-    <mergeCell ref="G104:I104"/>
-    <mergeCell ref="J104:L104"/>
-    <mergeCell ref="M104:O104"/>
-    <mergeCell ref="G101:I101"/>
-    <mergeCell ref="J101:L101"/>
-    <mergeCell ref="M101:O101"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="J102:L102"/>
-    <mergeCell ref="M102:O102"/>
-    <mergeCell ref="G107:I107"/>
-    <mergeCell ref="J107:L107"/>
-    <mergeCell ref="M107:O107"/>
-    <mergeCell ref="G108:I108"/>
-    <mergeCell ref="J108:L108"/>
-    <mergeCell ref="M108:O108"/>
-    <mergeCell ref="G105:I105"/>
-    <mergeCell ref="J105:L105"/>
-    <mergeCell ref="M105:O105"/>
-    <mergeCell ref="G106:I106"/>
-    <mergeCell ref="J106:L106"/>
-    <mergeCell ref="M106:O106"/>
-    <mergeCell ref="E111:I111"/>
-    <mergeCell ref="J111:L111"/>
-    <mergeCell ref="M111:O111"/>
-    <mergeCell ref="G109:I109"/>
-    <mergeCell ref="J109:L109"/>
-    <mergeCell ref="M109:O109"/>
-    <mergeCell ref="G110:I110"/>
-    <mergeCell ref="J110:L110"/>
-    <mergeCell ref="M110:O110"/>
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -6571,20 +6891,1483 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:S51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D19" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="H21" sqref="H21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="16.625" customWidth="1"/>
+    <col min="4" max="9" width="13.125" style="72" customWidth="1"/>
+    <col min="10" max="10" width="15.125" style="72" customWidth="1"/>
+    <col min="11" max="11" width="14.875" style="72" customWidth="1"/>
+    <col min="12" max="12" width="13.125" style="72" customWidth="1"/>
+    <col min="13" max="13" width="15.5" style="72" customWidth="1"/>
+    <col min="14" max="14" width="17.375" style="72" customWidth="1"/>
+    <col min="15" max="15" width="17" style="72" customWidth="1"/>
+    <col min="16" max="16" width="31.375" style="72" customWidth="1"/>
+    <col min="17" max="19" width="13.125" style="72" customWidth="1"/>
+    <col min="20" max="21" width="13.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="48.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C1" s="79" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="71" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" s="71" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="G1" s="71" t="s">
+        <v>228</v>
+      </c>
+      <c r="H1" s="71" t="s">
+        <v>229</v>
+      </c>
+      <c r="I1" s="86" t="s">
+        <v>230</v>
+      </c>
+      <c r="J1" s="71" t="s">
+        <v>231</v>
+      </c>
+      <c r="K1" s="71" t="s">
+        <v>232</v>
+      </c>
+      <c r="L1" s="71" t="s">
+        <v>233</v>
+      </c>
+      <c r="M1" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="N1" s="71" t="s">
+        <v>235</v>
+      </c>
+      <c r="O1" s="71" t="s">
+        <v>236</v>
+      </c>
+      <c r="P1" s="71" t="s">
+        <v>237</v>
+      </c>
+      <c r="Q1" s="71" t="s">
+        <v>238</v>
+      </c>
+      <c r="R1" s="71" t="s">
+        <v>239</v>
+      </c>
+      <c r="S1" s="71" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="81" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="82"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="84" t="s">
+        <v>242</v>
+      </c>
+      <c r="D2" s="83" t="s">
+        <v>241</v>
+      </c>
+      <c r="E2" s="83" t="s">
+        <v>241</v>
+      </c>
+      <c r="F2" s="85" t="s">
+        <v>243</v>
+      </c>
+      <c r="G2" s="85" t="s">
+        <v>244</v>
+      </c>
+      <c r="H2" s="85" t="s">
+        <v>255</v>
+      </c>
+      <c r="I2" s="87"/>
+      <c r="J2" s="85" t="s">
+        <v>245</v>
+      </c>
+      <c r="K2" s="85" t="s">
+        <v>246</v>
+      </c>
+      <c r="L2" s="85" t="s">
+        <v>247</v>
+      </c>
+      <c r="M2" s="85" t="s">
+        <v>248</v>
+      </c>
+      <c r="N2" s="85" t="s">
+        <v>249</v>
+      </c>
+      <c r="O2" s="85" t="s">
+        <v>250</v>
+      </c>
+      <c r="P2" s="85" t="s">
+        <v>251</v>
+      </c>
+      <c r="Q2" s="85" t="s">
+        <v>252</v>
+      </c>
+      <c r="R2" s="85" t="s">
+        <v>253</v>
+      </c>
+      <c r="S2" s="85" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="73">
+        <v>1</v>
+      </c>
+      <c r="B3" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="75"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="29"/>
+      <c r="J3" s="29"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="29"/>
+      <c r="N3" s="29"/>
+      <c r="O3" s="29"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="29"/>
+      <c r="R3" s="29"/>
+      <c r="S3" s="29"/>
+    </row>
+    <row r="4" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="76">
+        <v>2</v>
+      </c>
+      <c r="B4" s="74" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+    </row>
+    <row r="5" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="73">
+        <v>3</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29"/>
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29"/>
+      <c r="S5" s="29"/>
+    </row>
+    <row r="6" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="77">
+        <v>4</v>
+      </c>
+      <c r="B6" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="29"/>
+      <c r="R6" s="29"/>
+      <c r="S6" s="29"/>
+    </row>
+    <row r="7" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="76">
+        <v>5</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
+      <c r="K7" s="29"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
+      <c r="N7" s="29"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="29"/>
+      <c r="S7" s="29"/>
+    </row>
+    <row r="8" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="73">
+        <v>6</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="66" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="29"/>
+      <c r="I8" s="29"/>
+      <c r="J8" s="29"/>
+      <c r="K8" s="29"/>
+      <c r="L8" s="29"/>
+      <c r="M8" s="29"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="29"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="29"/>
+      <c r="S8" s="29"/>
+    </row>
+    <row r="9" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="73">
+        <v>7</v>
+      </c>
+      <c r="B9" s="74" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="66" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="29"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
+      <c r="K9" s="29"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="29"/>
+      <c r="N9" s="29"/>
+      <c r="O9" s="29"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="29"/>
+      <c r="R9" s="29"/>
+      <c r="S9" s="29"/>
+    </row>
+    <row r="10" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="73">
+        <v>8</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
+      <c r="G10" s="29"/>
+      <c r="H10" s="29"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="29"/>
+      <c r="K10" s="29"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="29"/>
+      <c r="N10" s="29"/>
+      <c r="O10" s="29"/>
+      <c r="P10" s="29"/>
+      <c r="Q10" s="29"/>
+      <c r="R10" s="29"/>
+      <c r="S10" s="29"/>
+    </row>
+    <row r="11" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="73">
+        <v>9</v>
+      </c>
+      <c r="B11" s="74" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="29"/>
+      <c r="J11" s="29"/>
+      <c r="K11" s="29"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="29"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="29"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="29"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+    </row>
+    <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="76">
+        <v>10</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="66" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
+      <c r="K12" s="29"/>
+      <c r="L12" s="29"/>
+      <c r="M12" s="29"/>
+      <c r="N12" s="29"/>
+      <c r="O12" s="29"/>
+      <c r="P12" s="29"/>
+      <c r="Q12" s="29"/>
+      <c r="R12" s="29"/>
+      <c r="S12" s="29"/>
+    </row>
+    <row r="13" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="73">
+        <v>11</v>
+      </c>
+      <c r="B13" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="66" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+      <c r="O13" s="29"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="29"/>
+      <c r="R13" s="29"/>
+      <c r="S13" s="29"/>
+    </row>
+    <row r="14" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="77">
+        <v>12</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>71</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="29"/>
+      <c r="I14" s="29"/>
+      <c r="J14" s="29"/>
+      <c r="K14" s="29"/>
+      <c r="L14" s="29"/>
+      <c r="M14" s="29"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="29"/>
+      <c r="P14" s="29"/>
+      <c r="Q14" s="29"/>
+      <c r="R14" s="29"/>
+      <c r="S14" s="29"/>
+    </row>
+    <row r="15" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="76">
+        <v>13</v>
+      </c>
+      <c r="B15" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="29"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="29"/>
+      <c r="J15" s="29"/>
+      <c r="K15" s="29"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
+      <c r="N15" s="29"/>
+      <c r="O15" s="29"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="29"/>
+      <c r="R15" s="29"/>
+      <c r="S15" s="29"/>
+    </row>
+    <row r="16" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="76">
+        <v>14</v>
+      </c>
+      <c r="B16" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C16" s="66" t="s">
+        <v>82</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+      <c r="M16" s="29"/>
+      <c r="N16" s="29"/>
+      <c r="O16" s="29"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="29"/>
+      <c r="R16" s="29"/>
+      <c r="S16" s="29"/>
+    </row>
+    <row r="17" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="76">
+        <v>15</v>
+      </c>
+      <c r="B17" s="74" t="s">
+        <v>86</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
+      <c r="O17" s="29"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="29"/>
+      <c r="R17" s="29"/>
+      <c r="S17" s="29"/>
+    </row>
+    <row r="18" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="76">
+        <v>16</v>
+      </c>
+      <c r="B18" s="74" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+      <c r="M18" s="29"/>
+      <c r="N18" s="29"/>
+      <c r="O18" s="29"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="29"/>
+      <c r="R18" s="29"/>
+      <c r="S18" s="29"/>
+    </row>
+    <row r="19" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="76">
+        <v>17</v>
+      </c>
+      <c r="B19" s="74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="29"/>
+      <c r="N19" s="29"/>
+      <c r="O19" s="29"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="29"/>
+      <c r="R19" s="29"/>
+      <c r="S19" s="29"/>
+    </row>
+    <row r="20" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="76">
+        <v>18</v>
+      </c>
+      <c r="B20" s="74" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="29"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="29"/>
+      <c r="K20" s="29"/>
+      <c r="L20" s="29"/>
+      <c r="M20" s="29"/>
+      <c r="N20" s="29"/>
+      <c r="O20" s="29"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="29"/>
+      <c r="R20" s="29"/>
+      <c r="S20" s="29"/>
+    </row>
+    <row r="21" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="77">
+        <v>19</v>
+      </c>
+      <c r="B21" s="74" t="s">
+        <v>101</v>
+      </c>
+      <c r="C21" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="29"/>
+      <c r="N21" s="29"/>
+      <c r="O21" s="29"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="29"/>
+      <c r="R21" s="29"/>
+      <c r="S21" s="29"/>
+    </row>
+    <row r="22" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="73">
+        <v>20</v>
+      </c>
+      <c r="B22" s="74" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="66" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+      <c r="S22" s="29"/>
+    </row>
+    <row r="23" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="73">
+        <v>21</v>
+      </c>
+      <c r="B23" s="74" t="s">
+        <v>109</v>
+      </c>
+      <c r="C23" s="66" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+    </row>
+    <row r="24" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="73">
+        <v>22</v>
+      </c>
+      <c r="B24" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="C24" s="67" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+      <c r="S24" s="29"/>
+    </row>
+    <row r="25" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="73">
+        <v>23</v>
+      </c>
+      <c r="B25" s="74" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="66" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+      <c r="S25" s="29"/>
+    </row>
+    <row r="26" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="73">
+        <v>24</v>
+      </c>
+      <c r="B26" s="74" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="66" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
+      <c r="M26" s="29"/>
+      <c r="N26" s="29"/>
+      <c r="O26" s="29"/>
+      <c r="P26" s="29"/>
+      <c r="Q26" s="29"/>
+      <c r="R26" s="29"/>
+      <c r="S26" s="29"/>
+    </row>
+    <row r="27" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="73">
+        <v>25</v>
+      </c>
+      <c r="B27" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="66" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
+      <c r="M27" s="29"/>
+      <c r="N27" s="29"/>
+      <c r="O27" s="29"/>
+      <c r="P27" s="29"/>
+      <c r="Q27" s="29"/>
+      <c r="R27" s="29"/>
+      <c r="S27" s="29"/>
+    </row>
+    <row r="28" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="73">
+        <v>26</v>
+      </c>
+      <c r="B28" s="74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C28" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="29"/>
+      <c r="N28" s="29"/>
+      <c r="O28" s="29"/>
+      <c r="P28" s="29"/>
+      <c r="Q28" s="29"/>
+      <c r="R28" s="29"/>
+      <c r="S28" s="29"/>
+    </row>
+    <row r="29" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="73">
+        <v>27</v>
+      </c>
+      <c r="B29" s="74" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+      <c r="L29" s="29"/>
+      <c r="M29" s="29"/>
+      <c r="N29" s="29"/>
+      <c r="O29" s="29"/>
+      <c r="P29" s="29"/>
+      <c r="Q29" s="29"/>
+      <c r="R29" s="29"/>
+      <c r="S29" s="29"/>
+    </row>
+    <row r="30" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="77">
+        <v>28</v>
+      </c>
+      <c r="B30" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+      <c r="L30" s="29"/>
+      <c r="M30" s="29"/>
+      <c r="N30" s="29"/>
+      <c r="O30" s="29"/>
+      <c r="P30" s="29"/>
+      <c r="Q30" s="29"/>
+      <c r="R30" s="29"/>
+      <c r="S30" s="29"/>
+    </row>
+    <row r="31" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="76">
+        <v>29</v>
+      </c>
+      <c r="B31" s="74" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" s="65" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+      <c r="L31" s="29"/>
+      <c r="M31" s="29"/>
+      <c r="N31" s="29"/>
+      <c r="O31" s="29"/>
+      <c r="P31" s="29"/>
+      <c r="Q31" s="29"/>
+      <c r="R31" s="29"/>
+      <c r="S31" s="29"/>
+    </row>
+    <row r="32" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="73">
+        <v>30</v>
+      </c>
+      <c r="B32" s="74" t="s">
+        <v>142</v>
+      </c>
+      <c r="C32" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+      <c r="L32" s="29"/>
+      <c r="M32" s="29"/>
+      <c r="N32" s="29"/>
+      <c r="O32" s="29"/>
+      <c r="P32" s="29"/>
+      <c r="Q32" s="29"/>
+      <c r="R32" s="29"/>
+      <c r="S32" s="29"/>
+    </row>
+    <row r="33" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="73">
+        <v>31</v>
+      </c>
+      <c r="B33" s="74" t="s">
+        <v>147</v>
+      </c>
+      <c r="C33" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+      <c r="L33" s="29"/>
+      <c r="M33" s="29"/>
+      <c r="N33" s="29"/>
+      <c r="O33" s="29"/>
+      <c r="P33" s="29"/>
+      <c r="Q33" s="29"/>
+      <c r="R33" s="29"/>
+      <c r="S33" s="29"/>
+    </row>
+    <row r="34" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="73">
+        <v>32</v>
+      </c>
+      <c r="B34" s="74" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+      <c r="L34" s="29"/>
+      <c r="M34" s="29"/>
+      <c r="N34" s="29"/>
+      <c r="O34" s="29"/>
+      <c r="P34" s="29"/>
+      <c r="Q34" s="29"/>
+      <c r="R34" s="29"/>
+      <c r="S34" s="29"/>
+    </row>
+    <row r="35" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="76">
+        <v>33</v>
+      </c>
+      <c r="B35" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="C35" s="69" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="29"/>
+      <c r="I35" s="29"/>
+      <c r="J35" s="29"/>
+      <c r="K35" s="29"/>
+      <c r="L35" s="29"/>
+      <c r="M35" s="29"/>
+      <c r="N35" s="29"/>
+      <c r="O35" s="29"/>
+      <c r="P35" s="29"/>
+      <c r="Q35" s="29"/>
+      <c r="R35" s="29"/>
+      <c r="S35" s="29"/>
+    </row>
+    <row r="36" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="73">
+        <v>34</v>
+      </c>
+      <c r="B36" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="C36" s="69" t="s">
+        <v>157</v>
+      </c>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="29"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="29"/>
+      <c r="I36" s="29"/>
+      <c r="J36" s="29"/>
+      <c r="K36" s="29"/>
+      <c r="L36" s="29"/>
+      <c r="M36" s="29"/>
+      <c r="N36" s="29"/>
+      <c r="O36" s="29"/>
+      <c r="P36" s="29"/>
+      <c r="Q36" s="29"/>
+      <c r="R36" s="29"/>
+      <c r="S36" s="29"/>
+    </row>
+    <row r="37" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="76">
+        <v>35</v>
+      </c>
+      <c r="B37" s="74" t="s">
+        <v>160</v>
+      </c>
+      <c r="C37" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="29"/>
+      <c r="I37" s="29"/>
+      <c r="J37" s="29"/>
+      <c r="K37" s="29"/>
+      <c r="L37" s="29"/>
+      <c r="M37" s="29"/>
+      <c r="N37" s="29"/>
+      <c r="O37" s="29"/>
+      <c r="P37" s="29"/>
+      <c r="Q37" s="29"/>
+      <c r="R37" s="29"/>
+      <c r="S37" s="29"/>
+    </row>
+    <row r="38" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="77">
+        <v>36</v>
+      </c>
+      <c r="B38" s="74" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="29"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="29"/>
+      <c r="I38" s="29"/>
+      <c r="J38" s="29"/>
+      <c r="K38" s="29"/>
+      <c r="L38" s="29"/>
+      <c r="M38" s="29"/>
+      <c r="N38" s="29"/>
+      <c r="O38" s="29"/>
+      <c r="P38" s="29"/>
+      <c r="Q38" s="29"/>
+      <c r="R38" s="29"/>
+      <c r="S38" s="29"/>
+    </row>
+    <row r="39" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="76">
+        <v>37</v>
+      </c>
+      <c r="B39" s="74" t="s">
+        <v>166</v>
+      </c>
+      <c r="C39" s="69" t="s">
+        <v>167</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="29"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="29"/>
+      <c r="I39" s="29"/>
+      <c r="J39" s="29"/>
+      <c r="K39" s="29"/>
+      <c r="L39" s="29"/>
+      <c r="M39" s="29"/>
+      <c r="N39" s="29"/>
+      <c r="O39" s="29"/>
+      <c r="P39" s="29"/>
+      <c r="Q39" s="29"/>
+      <c r="R39" s="29"/>
+      <c r="S39" s="29"/>
+    </row>
+    <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="73">
+        <v>38</v>
+      </c>
+      <c r="B40" s="74" t="s">
+        <v>169</v>
+      </c>
+      <c r="C40" s="69" t="s">
+        <v>170</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29"/>
+      <c r="F40" s="29"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="29"/>
+      <c r="I40" s="29"/>
+      <c r="J40" s="29"/>
+      <c r="K40" s="29"/>
+      <c r="L40" s="29"/>
+      <c r="M40" s="29"/>
+      <c r="N40" s="29"/>
+      <c r="O40" s="29"/>
+      <c r="P40" s="29"/>
+      <c r="Q40" s="29"/>
+      <c r="R40" s="29"/>
+      <c r="S40" s="29"/>
+    </row>
+    <row r="41" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="76">
+        <v>39</v>
+      </c>
+      <c r="B41" s="74" t="s">
+        <v>173</v>
+      </c>
+      <c r="C41" s="69" t="s">
+        <v>174</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="29"/>
+      <c r="I41" s="29"/>
+      <c r="J41" s="29"/>
+      <c r="K41" s="29"/>
+      <c r="L41" s="29"/>
+      <c r="M41" s="29"/>
+      <c r="N41" s="29"/>
+      <c r="O41" s="29"/>
+      <c r="P41" s="29"/>
+      <c r="Q41" s="29"/>
+      <c r="R41" s="29"/>
+      <c r="S41" s="29"/>
+    </row>
+    <row r="42" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="76">
+        <v>40</v>
+      </c>
+      <c r="B42" s="74" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="69" t="s">
+        <v>178</v>
+      </c>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="29"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
+      <c r="J42" s="29"/>
+      <c r="K42" s="29"/>
+      <c r="L42" s="29"/>
+      <c r="M42" s="29"/>
+      <c r="N42" s="29"/>
+      <c r="O42" s="29"/>
+      <c r="P42" s="29"/>
+      <c r="Q42" s="29"/>
+      <c r="R42" s="29"/>
+      <c r="S42" s="29"/>
+    </row>
+    <row r="43" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="76">
+        <v>41</v>
+      </c>
+      <c r="B43" s="74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C43" s="69" t="s">
+        <v>182</v>
+      </c>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29"/>
+      <c r="F43" s="29"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="29"/>
+      <c r="I43" s="29"/>
+      <c r="J43" s="29"/>
+      <c r="K43" s="29"/>
+      <c r="L43" s="29"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="29"/>
+      <c r="O43" s="29"/>
+      <c r="P43" s="29"/>
+      <c r="Q43" s="29"/>
+      <c r="R43" s="29"/>
+      <c r="S43" s="29"/>
+    </row>
+    <row r="44" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="76">
+        <v>42</v>
+      </c>
+      <c r="B44" s="74" t="s">
+        <v>184</v>
+      </c>
+      <c r="C44" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="29"/>
+      <c r="G44" s="29"/>
+      <c r="H44" s="29"/>
+      <c r="I44" s="29"/>
+      <c r="J44" s="29"/>
+      <c r="K44" s="29"/>
+      <c r="L44" s="29"/>
+      <c r="M44" s="29"/>
+      <c r="N44" s="29"/>
+      <c r="O44" s="29"/>
+      <c r="P44" s="29"/>
+      <c r="Q44" s="29"/>
+      <c r="R44" s="29"/>
+      <c r="S44" s="29"/>
+    </row>
+    <row r="45" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="76">
+        <v>43</v>
+      </c>
+      <c r="B45" s="74" t="s">
+        <v>188</v>
+      </c>
+      <c r="C45" s="69" t="s">
+        <v>189</v>
+      </c>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="29"/>
+      <c r="I45" s="29"/>
+      <c r="J45" s="29"/>
+      <c r="K45" s="29"/>
+      <c r="L45" s="29"/>
+      <c r="M45" s="29"/>
+      <c r="N45" s="29"/>
+      <c r="O45" s="29"/>
+      <c r="P45" s="29"/>
+      <c r="Q45" s="29"/>
+      <c r="R45" s="29"/>
+      <c r="S45" s="29"/>
+    </row>
+    <row r="46" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="73">
+        <v>44</v>
+      </c>
+      <c r="B46" s="74" t="s">
+        <v>191</v>
+      </c>
+      <c r="C46" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="29"/>
+      <c r="I46" s="29"/>
+      <c r="J46" s="29"/>
+      <c r="K46" s="29"/>
+      <c r="L46" s="29"/>
+      <c r="M46" s="29"/>
+      <c r="N46" s="29"/>
+      <c r="O46" s="29"/>
+      <c r="P46" s="29"/>
+      <c r="Q46" s="29"/>
+      <c r="R46" s="29"/>
+      <c r="S46" s="29"/>
+    </row>
+    <row r="47" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="73">
+        <v>45</v>
+      </c>
+      <c r="B47" s="74" t="s">
+        <v>195</v>
+      </c>
+      <c r="C47" s="65" t="s">
+        <v>196</v>
+      </c>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+    </row>
+    <row r="48" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="76">
+        <v>46</v>
+      </c>
+      <c r="B48" s="78" t="s">
+        <v>199</v>
+      </c>
+      <c r="C48" s="65" t="s">
+        <v>199</v>
+      </c>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="29"/>
+      <c r="I48" s="29"/>
+      <c r="J48" s="29"/>
+      <c r="K48" s="29"/>
+      <c r="L48" s="29"/>
+      <c r="M48" s="29"/>
+      <c r="N48" s="29"/>
+      <c r="O48" s="29"/>
+      <c r="P48" s="29"/>
+      <c r="Q48" s="29"/>
+      <c r="R48" s="29"/>
+      <c r="S48" s="29"/>
+    </row>
+    <row r="49" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="76">
+        <v>47</v>
+      </c>
+      <c r="B49" s="78" t="s">
+        <v>202</v>
+      </c>
+      <c r="C49" s="65" t="s">
+        <v>202</v>
+      </c>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29"/>
+      <c r="F49" s="29"/>
+      <c r="G49" s="29"/>
+      <c r="H49" s="29"/>
+      <c r="I49" s="29"/>
+      <c r="J49" s="29"/>
+      <c r="K49" s="29"/>
+      <c r="L49" s="29"/>
+      <c r="M49" s="29"/>
+      <c r="N49" s="29"/>
+      <c r="O49" s="29"/>
+      <c r="P49" s="29"/>
+      <c r="Q49" s="29"/>
+      <c r="R49" s="29"/>
+      <c r="S49" s="29"/>
+    </row>
+    <row r="50" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="77">
+        <v>48</v>
+      </c>
+      <c r="B50" s="78" t="s">
+        <v>205</v>
+      </c>
+      <c r="C50" s="65" t="s">
+        <v>205</v>
+      </c>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="29"/>
+      <c r="G50" s="29"/>
+      <c r="H50" s="29"/>
+      <c r="I50" s="29"/>
+      <c r="J50" s="29"/>
+      <c r="K50" s="29"/>
+      <c r="L50" s="29"/>
+      <c r="M50" s="29"/>
+      <c r="N50" s="29"/>
+      <c r="O50" s="29"/>
+      <c r="P50" s="29"/>
+      <c r="Q50" s="29"/>
+      <c r="R50" s="29"/>
+      <c r="S50" s="29"/>
+    </row>
+    <row r="51" spans="1:19" s="80" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="76">
+        <v>49</v>
+      </c>
+      <c r="B51" s="78" t="s">
+        <v>208</v>
+      </c>
+      <c r="C51" s="65" t="s">
+        <v>208</v>
+      </c>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="29"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="29"/>
+      <c r="K51" s="29"/>
+      <c r="L51" s="29"/>
+      <c r="M51" s="29"/>
+      <c r="N51" s="29"/>
+      <c r="O51" s="29"/>
+      <c r="P51" s="29"/>
+      <c r="Q51" s="29"/>
+      <c r="R51" s="29"/>
+      <c r="S51" s="29"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:K26"/>
   <sheetViews>
     <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B1" s="59" t="s">
-        <v>216</v>
-      </c>
-      <c r="C1" s="59"/>
+      <c r="B1" s="62" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="61"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -6595,8 +8378,8 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -6607,16 +8390,16 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B3" s="58" t="s">
+      <c r="B3" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="58"/>
+      <c r="C3" s="60"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.15">
-      <c r="B4" s="58" t="s">
+      <c r="B4" s="60" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="58"/>
+      <c r="C4" s="60"/>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B5" s="2"/>
@@ -6692,22 +8475,7 @@
   </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
-  <sheetData/>
-  <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
src edit 8.26 23:41 update id.v and inst.xlsx.
</commit_message>
<xml_diff>
--- a/指令.xlsx
+++ b/指令.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/38d7c1f78c795a43/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Code\cpu\bitmips_experiments-master\lab5\teach_soc\teach_soc.srcs\sources_1\new\myCPU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7CABB16E-B7C3-4FF5-A40D-6B679D9CC289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF3CD32-5C02-4A6C-A7CB-12FC895596ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32760" yWindow="32760" windowWidth="22365" windowHeight="9420" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="46080" windowHeight="21852" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="指令译码" sheetId="1" r:id="rId1"/>
@@ -18,23 +18,11 @@
     <sheet name="alu信号" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="326">
   <si>
     <t>指令</t>
   </si>
@@ -364,6 +352,8 @@
         <sz val="8"/>
         <color rgb="FF333333"/>
         <rFont val="微软雅黑"/>
+        <family val="2"/>
+        <charset val="134"/>
       </rPr>
       <t>立即数逻辑右移</t>
     </r>
@@ -1368,24 +1358,62 @@
     <t>imm16_signe + reg1_data_i</t>
   </si>
   <si>
+    <t>data_ram[reg1_o] = reg2_o
+byte</t>
+  </si>
+  <si>
+    <t>rt = data_ram[reg1_o + reg2_o]
+half word</t>
+  </si>
+  <si>
+    <t>data_ram[reg1_o] = reg2_o
+half word</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         alu信号
+指令</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
     <t>rt = data_ram[reg1_o + reg2_o]
 byte</t>
-  </si>
-  <si>
-    <t>data_ram[reg1_o] = reg2_o
-byte</t>
-  </si>
-  <si>
-    <t>rt = data_ram[reg1_o + reg2_o]
-half word</t>
-  </si>
-  <si>
-    <t>data_ram[reg1_o] = reg2_o
-half word</t>
-  </si>
-  <si>
-    <t xml:space="preserve">         alu信号
-指令</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>imm16_signe</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>rt = (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4F4F4F"/>
+        <rFont val="微软雅黑"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">无符号比较 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4F4F4F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>reg1_o &lt; reg2_o) ? 1 : 0</t>
+    </r>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>`ZeroWord</t>
+    <phoneticPr fontId="15" type="noConversion"/>
+  </si>
+  <si>
+    <t>`ReadEnable</t>
     <phoneticPr fontId="15" type="noConversion"/>
   </si>
 </sst>
@@ -1393,7 +1421,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="28">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -1549,6 +1577,8 @@
       <sz val="8"/>
       <color rgb="FF333333"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="8"/>
@@ -1560,6 +1590,13 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4F4F4F"/>
+      <name val="微软雅黑"/>
+      <family val="3"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="10">
@@ -2068,77 +2105,161 @@
     <xf numFmtId="0" fontId="20" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="27" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="18" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2148,90 +2269,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="27" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="6" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="18" fillId="6" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="4" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2511,18 +2548,18 @@
   <dimension ref="A1:S111"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D36" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="M44" sqref="M44:O44"/>
-      <selection pane="bottomLeft"/>
-      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="15" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="22.5">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B1" s="2"/>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -2545,13 +2582,13 @@
       <c r="I1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="55" t="s">
+      <c r="J1" s="94" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-    </row>
-    <row r="2" spans="1:19" ht="54">
+      <c r="K1" s="95"/>
+      <c r="L1" s="95"/>
+    </row>
+    <row r="2" spans="1:19" ht="57.6" x14ac:dyDescent="0.25">
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
         <v>8</v>
@@ -2577,9 +2614,9 @@
       <c r="J2" s="24"/>
       <c r="K2" s="3"/>
       <c r="L2" s="25"/>
-      <c r="M2" s="106"/>
-      <c r="N2" s="106"/>
-      <c r="O2" s="106"/>
+      <c r="M2" s="96"/>
+      <c r="N2" s="96"/>
+      <c r="O2" s="96"/>
       <c r="P2" s="25"/>
       <c r="Q2" s="25"/>
       <c r="R2" s="25"/>
@@ -2587,7 +2624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -2606,21 +2643,21 @@
       <c r="F3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="58"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="60" t="s">
+      <c r="H3" s="61"/>
+      <c r="I3" s="62"/>
+      <c r="J3" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="82" t="s">
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="82"/>
-      <c r="O3" s="82"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
       <c r="P3" s="26"/>
       <c r="Q3" s="26"/>
       <c r="R3" s="26"/>
@@ -2628,7 +2665,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2647,21 +2684,21 @@
       <c r="F4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="58"/>
-      <c r="I4" s="59"/>
-      <c r="J4" s="60" t="s">
+      <c r="H4" s="61"/>
+      <c r="I4" s="62"/>
+      <c r="J4" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="82" t="s">
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="82"/>
-      <c r="O4" s="82"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
       <c r="P4" s="26"/>
       <c r="Q4" s="26"/>
       <c r="R4" s="26"/>
@@ -2669,7 +2706,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -2688,21 +2725,21 @@
       <c r="F5" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="58"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="60" t="s">
+      <c r="H5" s="61"/>
+      <c r="I5" s="62"/>
+      <c r="J5" s="63" t="s">
         <v>32</v>
       </c>
-      <c r="K5" s="60"/>
-      <c r="L5" s="60"/>
-      <c r="M5" s="82" t="s">
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="N5" s="82"/>
-      <c r="O5" s="82"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
       <c r="P5" s="26"/>
       <c r="Q5" s="26"/>
       <c r="R5" s="26"/>
@@ -2710,7 +2747,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="30">
         <v>4</v>
       </c>
@@ -2738,16 +2775,16 @@
       <c r="I6" s="11">
         <v>100100</v>
       </c>
-      <c r="J6" s="60" t="s">
+      <c r="J6" s="63" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="60"/>
-      <c r="L6" s="60"/>
-      <c r="M6" s="82" t="s">
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="82"/>
-      <c r="O6" s="82"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
       <c r="P6" s="26"/>
       <c r="Q6" s="26"/>
       <c r="R6" s="26"/>
@@ -2755,7 +2792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -2783,14 +2820,14 @@
       <c r="I7" s="11">
         <v>100111</v>
       </c>
-      <c r="J7" s="107"/>
-      <c r="K7" s="107"/>
-      <c r="L7" s="107"/>
-      <c r="M7" s="82" t="s">
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="N7" s="82"/>
-      <c r="O7" s="82"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
       <c r="P7" s="26"/>
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
@@ -2798,7 +2835,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>6</v>
       </c>
@@ -2826,16 +2863,16 @@
       <c r="I8" s="11">
         <v>100101</v>
       </c>
-      <c r="J8" s="60" t="s">
+      <c r="J8" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="82" t="s">
+      <c r="K8" s="63"/>
+      <c r="L8" s="63"/>
+      <c r="M8" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="N8" s="82"/>
-      <c r="O8" s="82"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
       <c r="P8" s="26"/>
       <c r="Q8" s="26"/>
       <c r="R8" s="26"/>
@@ -2843,7 +2880,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -2871,16 +2908,16 @@
       <c r="I9" s="11">
         <v>100110</v>
       </c>
-      <c r="J9" s="60" t="s">
+      <c r="J9" s="63" t="s">
         <v>50</v>
       </c>
-      <c r="K9" s="60"/>
-      <c r="L9" s="60"/>
-      <c r="M9" s="82" t="s">
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
       <c r="P9" s="26"/>
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
@@ -2888,7 +2925,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:19">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>8</v>
       </c>
@@ -2907,21 +2944,21 @@
       <c r="F10" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="58"/>
-      <c r="I10" s="59"/>
-      <c r="J10" s="62" t="s">
+      <c r="H10" s="61"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="58" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="62"/>
-      <c r="L10" s="62"/>
-      <c r="M10" s="82" t="s">
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="69" t="s">
         <v>56</v>
       </c>
-      <c r="N10" s="82"/>
-      <c r="O10" s="82"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
       <c r="P10" s="26"/>
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
@@ -2929,7 +2966,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:19">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -2957,16 +2994,16 @@
       <c r="I11" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="63" t="s">
+      <c r="J11" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="K11" s="63"/>
-      <c r="L11" s="63"/>
-      <c r="M11" s="82" t="s">
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="N11" s="82"/>
-      <c r="O11" s="82"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="69"/>
       <c r="P11" s="26"/>
       <c r="Q11" s="26"/>
       <c r="R11" s="26"/>
@@ -2974,7 +3011,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:19">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3002,16 +3039,16 @@
       <c r="I12" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="J12" s="64" t="s">
+      <c r="J12" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="82" t="s">
+      <c r="K12" s="65"/>
+      <c r="L12" s="65"/>
+      <c r="M12" s="69" t="s">
         <v>66</v>
       </c>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
       <c r="P12" s="26"/>
       <c r="Q12" s="26"/>
       <c r="R12" s="26"/>
@@ -3019,7 +3056,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -3047,16 +3084,16 @@
       <c r="I13" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="J13" s="95" t="s">
+      <c r="J13" s="93" t="s">
         <v>70</v>
       </c>
-      <c r="K13" s="62"/>
-      <c r="L13" s="62"/>
-      <c r="M13" s="83" t="s">
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="N13" s="83"/>
-      <c r="O13" s="83"/>
+      <c r="N13" s="70"/>
+      <c r="O13" s="70"/>
       <c r="P13" s="26"/>
       <c r="Q13" s="26"/>
       <c r="R13" s="26"/>
@@ -3064,7 +3101,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:19">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="30">
         <v>12</v>
       </c>
@@ -3092,16 +3129,16 @@
       <c r="I14" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="J14" s="64" t="s">
+      <c r="J14" s="65" t="s">
         <v>75</v>
       </c>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="82" t="s">
+      <c r="K14" s="65"/>
+      <c r="L14" s="65"/>
+      <c r="M14" s="69" t="s">
         <v>76</v>
       </c>
-      <c r="N14" s="82"/>
-      <c r="O14" s="82"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="69"/>
       <c r="P14" s="26"/>
       <c r="Q14" s="26"/>
       <c r="R14" s="26"/>
@@ -3109,7 +3146,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -3137,16 +3174,16 @@
       <c r="I15" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="J15" s="64" t="s">
+      <c r="J15" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="82" t="s">
+      <c r="K15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15" s="69" t="s">
         <v>81</v>
       </c>
-      <c r="N15" s="82"/>
-      <c r="O15" s="82"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
       <c r="P15" s="26"/>
       <c r="Q15" s="26"/>
       <c r="R15" s="26"/>
@@ -3154,7 +3191,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:19">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -3182,16 +3219,16 @@
       <c r="I16" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="J16" s="64" t="s">
+      <c r="J16" s="65" t="s">
         <v>85</v>
       </c>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="82" t="s">
+      <c r="K16" s="65"/>
+      <c r="L16" s="65"/>
+      <c r="M16" s="69" t="s">
         <v>86</v>
       </c>
-      <c r="N16" s="82"/>
-      <c r="O16" s="82"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="69"/>
       <c r="P16" s="26"/>
       <c r="Q16" s="26"/>
       <c r="R16" s="26"/>
@@ -3199,7 +3236,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:19">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -3227,11 +3264,11 @@
       <c r="I17" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J17" s="66" t="s">
+      <c r="J17" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="K17" s="67"/>
-      <c r="L17" s="68"/>
+      <c r="K17" s="91"/>
+      <c r="L17" s="92"/>
       <c r="M17" s="84"/>
       <c r="N17" s="85"/>
       <c r="O17" s="86"/>
@@ -3242,7 +3279,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:19">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -3270,11 +3307,11 @@
       <c r="I18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J18" s="66" t="s">
+      <c r="J18" s="90" t="s">
         <v>93</v>
       </c>
-      <c r="K18" s="67"/>
-      <c r="L18" s="68"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="92"/>
       <c r="M18" s="84"/>
       <c r="N18" s="85"/>
       <c r="O18" s="86"/>
@@ -3285,7 +3322,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:19">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3313,11 +3350,11 @@
       <c r="I19" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="J19" s="66" t="s">
+      <c r="J19" s="90" t="s">
         <v>96</v>
       </c>
-      <c r="K19" s="67"/>
-      <c r="L19" s="68"/>
+      <c r="K19" s="91"/>
+      <c r="L19" s="92"/>
       <c r="M19" s="84"/>
       <c r="N19" s="85"/>
       <c r="O19" s="86"/>
@@ -3328,7 +3365,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:19">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3356,24 +3393,24 @@
       <c r="I20" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="J20" s="70"/>
-      <c r="K20" s="71"/>
-      <c r="L20" s="72"/>
+      <c r="J20" s="81"/>
+      <c r="K20" s="82"/>
+      <c r="L20" s="83"/>
       <c r="M20" s="84" t="s">
         <v>100</v>
       </c>
       <c r="N20" s="85"/>
       <c r="O20" s="86"/>
-      <c r="P20" s="73" t="s">
+      <c r="P20" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="Q20" s="74"/>
-      <c r="R20" s="75"/>
+      <c r="Q20" s="88"/>
+      <c r="R20" s="89"/>
       <c r="S20" s="28">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="30">
         <v>19</v>
       </c>
@@ -3401,9 +3438,9 @@
       <c r="I21" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="J21" s="70"/>
-      <c r="K21" s="71"/>
-      <c r="L21" s="72"/>
+      <c r="J21" s="81"/>
+      <c r="K21" s="82"/>
+      <c r="L21" s="83"/>
       <c r="M21" s="84" t="s">
         <v>105</v>
       </c>
@@ -3416,7 +3453,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>20</v>
       </c>
@@ -3444,16 +3481,16 @@
       <c r="I22" s="27">
         <v>100000</v>
       </c>
-      <c r="J22" s="62" t="s">
+      <c r="J22" s="58" t="s">
         <v>108</v>
       </c>
-      <c r="K22" s="62"/>
-      <c r="L22" s="62"/>
-      <c r="M22" s="82" t="s">
+      <c r="K22" s="58"/>
+      <c r="L22" s="58"/>
+      <c r="M22" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="69"/>
       <c r="P22" s="26"/>
       <c r="Q22" s="26"/>
       <c r="R22" s="26"/>
@@ -3461,7 +3498,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
@@ -3489,14 +3526,14 @@
       <c r="I23" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="J23" s="107"/>
-      <c r="K23" s="107"/>
-      <c r="L23" s="107"/>
-      <c r="M23" s="82" t="s">
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="69" t="s">
         <v>109</v>
       </c>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
+      <c r="N23" s="69"/>
+      <c r="O23" s="69"/>
       <c r="P23" s="26"/>
       <c r="Q23" s="26"/>
       <c r="R23" s="26"/>
@@ -3504,7 +3541,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:19">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>22</v>
       </c>
@@ -3532,16 +3569,16 @@
       <c r="I24" s="11">
         <v>100010</v>
       </c>
-      <c r="J24" s="60" t="s">
+      <c r="J24" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="K24" s="60"/>
-      <c r="L24" s="60"/>
-      <c r="M24" s="82" t="s">
+      <c r="K24" s="63"/>
+      <c r="L24" s="63"/>
+      <c r="M24" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="N24" s="82"/>
-      <c r="O24" s="82"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
       <c r="P24" s="26"/>
       <c r="Q24" s="26"/>
       <c r="R24" s="26"/>
@@ -3549,7 +3586,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14.25" customHeight="1">
+    <row r="25" spans="1:19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>23</v>
       </c>
@@ -3577,14 +3614,14 @@
       <c r="I25" s="11">
         <v>100011</v>
       </c>
-      <c r="J25" s="107"/>
-      <c r="K25" s="107"/>
-      <c r="L25" s="107"/>
-      <c r="M25" s="82" t="s">
+      <c r="J25" s="64"/>
+      <c r="K25" s="64"/>
+      <c r="L25" s="64"/>
+      <c r="M25" s="69" t="s">
         <v>116</v>
       </c>
-      <c r="N25" s="82"/>
-      <c r="O25" s="82"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
       <c r="P25" s="26"/>
       <c r="Q25" s="26"/>
       <c r="R25" s="26"/>
@@ -3592,7 +3629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:19">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>24</v>
       </c>
@@ -3620,22 +3657,22 @@
       <c r="I26" s="11">
         <v>101010</v>
       </c>
-      <c r="J26" s="107"/>
-      <c r="K26" s="107"/>
-      <c r="L26" s="107"/>
-      <c r="M26" s="82" t="s">
+      <c r="J26" s="64"/>
+      <c r="K26" s="64"/>
+      <c r="L26" s="64"/>
+      <c r="M26" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="N26" s="82"/>
-      <c r="O26" s="82"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
+      <c r="N26" s="69"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
       <c r="S26" s="28">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
@@ -3663,22 +3700,22 @@
       <c r="I27" s="11">
         <v>101011</v>
       </c>
-      <c r="J27" s="107"/>
-      <c r="K27" s="107"/>
-      <c r="L27" s="107"/>
-      <c r="M27" s="82" t="s">
+      <c r="J27" s="64"/>
+      <c r="K27" s="64"/>
+      <c r="L27" s="64"/>
+      <c r="M27" s="69" t="s">
         <v>124</v>
       </c>
-      <c r="N27" s="82"/>
-      <c r="O27" s="82"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
       <c r="S27">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>26</v>
       </c>
@@ -3697,29 +3734,29 @@
       <c r="F28" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G28" s="57" t="s">
+      <c r="G28" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H28" s="58"/>
-      <c r="I28" s="59"/>
-      <c r="J28" s="60" t="s">
+      <c r="H28" s="61"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="K28" s="60"/>
-      <c r="L28" s="60"/>
-      <c r="M28" s="82" t="s">
+      <c r="K28" s="63"/>
+      <c r="L28" s="63"/>
+      <c r="M28" s="69" t="s">
         <v>129</v>
       </c>
-      <c r="N28" s="82"/>
-      <c r="O28" s="82"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="61"/>
-      <c r="R28" s="61"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
       <c r="S28" s="28">
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
@@ -3738,29 +3775,29 @@
       <c r="F29" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="57" t="s">
+      <c r="G29" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H29" s="58"/>
-      <c r="I29" s="59"/>
-      <c r="J29" s="108" t="s">
+      <c r="H29" s="61"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="K29" s="108"/>
-      <c r="L29" s="108"/>
-      <c r="M29" s="87" t="s">
+      <c r="K29" s="66"/>
+      <c r="L29" s="66"/>
+      <c r="M29" s="80" t="s">
         <v>134</v>
       </c>
-      <c r="N29" s="87"/>
-      <c r="O29" s="87"/>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="65"/>
-      <c r="R29" s="65"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="80"/>
+      <c r="P29" s="67"/>
+      <c r="Q29" s="67"/>
+      <c r="R29" s="67"/>
       <c r="S29">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="30">
         <v>28</v>
       </c>
@@ -3779,27 +3816,27 @@
       <c r="F30" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G30" s="57" t="s">
+      <c r="G30" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H30" s="58"/>
-      <c r="I30" s="59"/>
-      <c r="J30" s="107"/>
-      <c r="K30" s="107"/>
-      <c r="L30" s="109"/>
-      <c r="M30" s="88" t="s">
+      <c r="H30" s="61"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="72"/>
+      <c r="M30" s="73" t="s">
         <v>137</v>
       </c>
-      <c r="N30" s="89"/>
-      <c r="O30" s="90"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="61"/>
-      <c r="R30" s="61"/>
+      <c r="N30" s="74"/>
+      <c r="O30" s="75"/>
+      <c r="P30" s="76"/>
+      <c r="Q30" s="59"/>
+      <c r="R30" s="59"/>
       <c r="S30" s="28">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -3818,27 +3855,27 @@
       <c r="F31" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="57" t="s">
+      <c r="G31" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H31" s="58"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="107"/>
-      <c r="K31" s="107"/>
-      <c r="L31" s="109"/>
-      <c r="M31" s="91" t="s">
+      <c r="H31" s="61"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="72"/>
+      <c r="M31" s="77" t="s">
         <v>140</v>
       </c>
-      <c r="N31" s="92"/>
-      <c r="O31" s="93"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="61"/>
+      <c r="N31" s="78"/>
+      <c r="O31" s="79"/>
+      <c r="P31" s="76"/>
+      <c r="Q31" s="59"/>
+      <c r="R31" s="59"/>
       <c r="S31">
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>30</v>
       </c>
@@ -3851,31 +3888,31 @@
       <c r="D32" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E32" s="76" t="s">
+      <c r="E32" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="F32" s="77"/>
-      <c r="G32" s="77"/>
-      <c r="H32" s="77"/>
-      <c r="I32" s="78"/>
-      <c r="J32" s="62" t="s">
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="K32" s="62"/>
-      <c r="L32" s="62"/>
-      <c r="M32" s="94" t="s">
+      <c r="K32" s="58"/>
+      <c r="L32" s="58"/>
+      <c r="M32" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="N32" s="94"/>
-      <c r="O32" s="94"/>
-      <c r="P32" s="61"/>
-      <c r="Q32" s="61"/>
-      <c r="R32" s="61"/>
+      <c r="N32" s="71"/>
+      <c r="O32" s="71"/>
+      <c r="P32" s="59"/>
+      <c r="Q32" s="59"/>
+      <c r="R32" s="59"/>
       <c r="S32" s="28">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:19">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>31</v>
       </c>
@@ -3888,29 +3925,29 @@
       <c r="D33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E33" s="76" t="s">
+      <c r="E33" s="55" t="s">
         <v>143</v>
       </c>
-      <c r="F33" s="77"/>
-      <c r="G33" s="77"/>
-      <c r="H33" s="77"/>
-      <c r="I33" s="78"/>
-      <c r="J33" s="107"/>
-      <c r="K33" s="107"/>
-      <c r="L33" s="107"/>
-      <c r="M33" s="82" t="s">
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="64"/>
+      <c r="K33" s="64"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="69" t="s">
         <v>148</v>
       </c>
-      <c r="N33" s="82"/>
-      <c r="O33" s="82"/>
-      <c r="P33" s="61"/>
-      <c r="Q33" s="61"/>
-      <c r="R33" s="61"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="59"/>
+      <c r="Q33" s="59"/>
+      <c r="R33" s="59"/>
       <c r="S33">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:19">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>32</v>
       </c>
@@ -3938,22 +3975,22 @@
       <c r="I34" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="J34" s="60"/>
-      <c r="K34" s="60"/>
-      <c r="L34" s="60"/>
-      <c r="M34" s="82" t="s">
+      <c r="J34" s="63"/>
+      <c r="K34" s="63"/>
+      <c r="L34" s="63"/>
+      <c r="M34" s="69" t="s">
         <v>151</v>
       </c>
-      <c r="N34" s="82"/>
-      <c r="O34" s="82"/>
-      <c r="P34" s="61"/>
-      <c r="Q34" s="61"/>
-      <c r="R34" s="61"/>
+      <c r="N34" s="69"/>
+      <c r="O34" s="69"/>
+      <c r="P34" s="59"/>
+      <c r="Q34" s="59"/>
+      <c r="R34" s="59"/>
       <c r="S34" s="28">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:19">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3981,22 +4018,22 @@
       <c r="I35" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="J35" s="62"/>
-      <c r="K35" s="62"/>
-      <c r="L35" s="62"/>
-      <c r="M35" s="82" t="s">
+      <c r="J35" s="58"/>
+      <c r="K35" s="58"/>
+      <c r="L35" s="58"/>
+      <c r="M35" s="69" t="s">
         <v>154</v>
       </c>
-      <c r="N35" s="82"/>
-      <c r="O35" s="82"/>
-      <c r="P35" s="61"/>
-      <c r="Q35" s="61"/>
-      <c r="R35" s="61"/>
+      <c r="N35" s="69"/>
+      <c r="O35" s="69"/>
+      <c r="P35" s="59"/>
+      <c r="Q35" s="59"/>
+      <c r="R35" s="59"/>
       <c r="S35">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:19">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>34</v>
       </c>
@@ -4015,27 +4052,27 @@
       <c r="F36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G36" s="57" t="s">
+      <c r="G36" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H36" s="58"/>
-      <c r="I36" s="59"/>
-      <c r="J36" s="107"/>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
-      <c r="M36" s="82" t="s">
+      <c r="H36" s="61"/>
+      <c r="I36" s="62"/>
+      <c r="J36" s="64"/>
+      <c r="K36" s="64"/>
+      <c r="L36" s="64"/>
+      <c r="M36" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="N36" s="82"/>
-      <c r="O36" s="82"/>
-      <c r="P36" s="61"/>
-      <c r="Q36" s="61"/>
-      <c r="R36" s="61"/>
+      <c r="N36" s="69"/>
+      <c r="O36" s="69"/>
+      <c r="P36" s="59"/>
+      <c r="Q36" s="59"/>
+      <c r="R36" s="59"/>
       <c r="S36" s="28">
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4054,27 +4091,27 @@
       <c r="F37" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="57" t="s">
+      <c r="G37" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H37" s="58"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="60"/>
-      <c r="K37" s="60"/>
-      <c r="L37" s="60"/>
-      <c r="M37" s="82" t="s">
+      <c r="H37" s="61"/>
+      <c r="I37" s="62"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
+      <c r="L37" s="63"/>
+      <c r="M37" s="69" t="s">
         <v>161</v>
       </c>
-      <c r="N37" s="82"/>
-      <c r="O37" s="82"/>
-      <c r="P37" s="61"/>
-      <c r="Q37" s="61"/>
-      <c r="R37" s="61"/>
+      <c r="N37" s="69"/>
+      <c r="O37" s="69"/>
+      <c r="P37" s="59"/>
+      <c r="Q37" s="59"/>
+      <c r="R37" s="59"/>
       <c r="S37">
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="30">
         <v>36</v>
       </c>
@@ -4093,27 +4130,27 @@
       <c r="F38" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="57" t="s">
+      <c r="G38" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H38" s="58"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="107"/>
-      <c r="K38" s="107"/>
-      <c r="L38" s="107"/>
-      <c r="M38" s="83" t="s">
+      <c r="H38" s="61"/>
+      <c r="I38" s="62"/>
+      <c r="J38" s="64"/>
+      <c r="K38" s="64"/>
+      <c r="L38" s="64"/>
+      <c r="M38" s="70" t="s">
         <v>164</v>
       </c>
-      <c r="N38" s="83"/>
-      <c r="O38" s="83"/>
-      <c r="P38" s="65"/>
-      <c r="Q38" s="65"/>
-      <c r="R38" s="65"/>
+      <c r="N38" s="70"/>
+      <c r="O38" s="70"/>
+      <c r="P38" s="67"/>
+      <c r="Q38" s="67"/>
+      <c r="R38" s="67"/>
       <c r="S38" s="28">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4132,27 +4169,27 @@
       <c r="F39" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G39" s="57" t="s">
+      <c r="G39" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H39" s="58"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="107"/>
-      <c r="K39" s="107"/>
-      <c r="L39" s="107"/>
-      <c r="M39" s="82" t="s">
+      <c r="H39" s="61"/>
+      <c r="I39" s="62"/>
+      <c r="J39" s="64"/>
+      <c r="K39" s="64"/>
+      <c r="L39" s="64"/>
+      <c r="M39" s="69" t="s">
         <v>167</v>
       </c>
-      <c r="N39" s="82"/>
-      <c r="O39" s="82"/>
-      <c r="P39" s="61"/>
-      <c r="Q39" s="61"/>
-      <c r="R39" s="61"/>
+      <c r="N39" s="69"/>
+      <c r="O39" s="69"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="59"/>
+      <c r="R39" s="59"/>
       <c r="S39">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:19">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>38</v>
       </c>
@@ -4171,27 +4208,27 @@
       <c r="F40" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G40" s="57" t="s">
+      <c r="G40" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H40" s="58"/>
-      <c r="I40" s="59"/>
-      <c r="J40" s="107"/>
-      <c r="K40" s="107"/>
-      <c r="L40" s="107"/>
-      <c r="M40" s="82" t="s">
+      <c r="H40" s="61"/>
+      <c r="I40" s="62"/>
+      <c r="J40" s="64"/>
+      <c r="K40" s="64"/>
+      <c r="L40" s="64"/>
+      <c r="M40" s="69" t="s">
         <v>171</v>
       </c>
-      <c r="N40" s="82"/>
-      <c r="O40" s="82"/>
-      <c r="P40" s="61"/>
-      <c r="Q40" s="61"/>
-      <c r="R40" s="61"/>
+      <c r="N40" s="69"/>
+      <c r="O40" s="69"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="59"/>
+      <c r="R40" s="59"/>
       <c r="S40" s="28">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:19">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4210,27 +4247,27 @@
       <c r="F41" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G41" s="57" t="s">
+      <c r="G41" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H41" s="58"/>
-      <c r="I41" s="59"/>
-      <c r="J41" s="60"/>
-      <c r="K41" s="60"/>
-      <c r="L41" s="60"/>
-      <c r="M41" s="82" t="s">
+      <c r="H41" s="61"/>
+      <c r="I41" s="62"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
+      <c r="L41" s="63"/>
+      <c r="M41" s="69" t="s">
         <v>175</v>
       </c>
-      <c r="N41" s="82"/>
-      <c r="O41" s="82"/>
-      <c r="P41" s="61"/>
-      <c r="Q41" s="61"/>
-      <c r="R41" s="61"/>
+      <c r="N41" s="69"/>
+      <c r="O41" s="69"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="59"/>
+      <c r="R41" s="59"/>
       <c r="S41">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:19">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4249,27 +4286,27 @@
       <c r="F42" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="G42" s="57" t="s">
+      <c r="G42" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H42" s="58"/>
-      <c r="I42" s="59"/>
-      <c r="J42" s="107"/>
-      <c r="K42" s="107"/>
-      <c r="L42" s="107"/>
-      <c r="M42" s="82" t="s">
+      <c r="H42" s="61"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="64"/>
+      <c r="K42" s="64"/>
+      <c r="L42" s="64"/>
+      <c r="M42" s="69" t="s">
         <v>179</v>
       </c>
-      <c r="N42" s="82"/>
-      <c r="O42" s="82"/>
-      <c r="P42" s="61"/>
-      <c r="Q42" s="61"/>
-      <c r="R42" s="61"/>
+      <c r="N42" s="69"/>
+      <c r="O42" s="69"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="59"/>
+      <c r="R42" s="59"/>
       <c r="S42" s="28">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4288,27 +4325,27 @@
       <c r="F43" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G43" s="57" t="s">
+      <c r="G43" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H43" s="58"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="60"/>
-      <c r="K43" s="60"/>
-      <c r="L43" s="60"/>
-      <c r="M43" s="82" t="s">
+      <c r="H43" s="61"/>
+      <c r="I43" s="62"/>
+      <c r="J43" s="63"/>
+      <c r="K43" s="63"/>
+      <c r="L43" s="63"/>
+      <c r="M43" s="69" t="s">
         <v>182</v>
       </c>
-      <c r="N43" s="82"/>
-      <c r="O43" s="82"/>
-      <c r="P43" s="61"/>
-      <c r="Q43" s="61"/>
-      <c r="R43" s="61"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="69"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="59"/>
+      <c r="R43" s="59"/>
       <c r="S43">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4327,27 +4364,27 @@
       <c r="F44" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="G44" s="57" t="s">
+      <c r="G44" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H44" s="58"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="60"/>
-      <c r="K44" s="60"/>
-      <c r="L44" s="60"/>
-      <c r="M44" s="82" t="s">
+      <c r="H44" s="61"/>
+      <c r="I44" s="62"/>
+      <c r="J44" s="63"/>
+      <c r="K44" s="63"/>
+      <c r="L44" s="63"/>
+      <c r="M44" s="69" t="s">
         <v>186</v>
       </c>
-      <c r="N44" s="82"/>
-      <c r="O44" s="82"/>
-      <c r="P44" s="61"/>
-      <c r="Q44" s="61"/>
-      <c r="R44" s="61"/>
+      <c r="N44" s="69"/>
+      <c r="O44" s="69"/>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="59"/>
+      <c r="R44" s="59"/>
       <c r="S44" s="28">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4366,27 +4403,27 @@
       <c r="F45" s="11" t="s">
         <v>185</v>
       </c>
-      <c r="G45" s="57" t="s">
+      <c r="G45" s="60" t="s">
         <v>157</v>
       </c>
-      <c r="H45" s="58"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="82" t="s">
+      <c r="H45" s="61"/>
+      <c r="I45" s="62"/>
+      <c r="J45" s="68"/>
+      <c r="K45" s="68"/>
+      <c r="L45" s="68"/>
+      <c r="M45" s="69" t="s">
         <v>189</v>
       </c>
-      <c r="N45" s="82"/>
-      <c r="O45" s="82"/>
-      <c r="P45" s="61"/>
-      <c r="Q45" s="61"/>
-      <c r="R45" s="61"/>
+      <c r="N45" s="69"/>
+      <c r="O45" s="69"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="59"/>
+      <c r="R45" s="59"/>
       <c r="S45">
         <v>43</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44</v>
       </c>
@@ -4405,29 +4442,29 @@
       <c r="F46" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G46" s="57" t="s">
+      <c r="G46" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H46" s="58"/>
-      <c r="I46" s="59"/>
-      <c r="J46" s="62" t="s">
+      <c r="H46" s="61"/>
+      <c r="I46" s="62"/>
+      <c r="J46" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="K46" s="62"/>
-      <c r="L46" s="62"/>
-      <c r="M46" s="82" t="s">
+      <c r="K46" s="58"/>
+      <c r="L46" s="58"/>
+      <c r="M46" s="69" t="s">
         <v>193</v>
       </c>
-      <c r="N46" s="82"/>
-      <c r="O46" s="82"/>
-      <c r="P46" s="61"/>
-      <c r="Q46" s="61"/>
-      <c r="R46" s="61"/>
+      <c r="N46" s="69"/>
+      <c r="O46" s="69"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="59"/>
+      <c r="R46" s="59"/>
       <c r="S46" s="28">
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>45</v>
       </c>
@@ -4446,29 +4483,29 @@
       <c r="F47" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="57" t="s">
+      <c r="G47" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H47" s="58"/>
-      <c r="I47" s="59"/>
-      <c r="J47" s="62" t="s">
+      <c r="H47" s="61"/>
+      <c r="I47" s="62"/>
+      <c r="J47" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="K47" s="62"/>
-      <c r="L47" s="62"/>
-      <c r="M47" s="82" t="s">
+      <c r="K47" s="58"/>
+      <c r="L47" s="58"/>
+      <c r="M47" s="69" t="s">
         <v>197</v>
       </c>
-      <c r="N47" s="82"/>
-      <c r="O47" s="82"/>
-      <c r="P47" s="61"/>
-      <c r="Q47" s="61"/>
-      <c r="R47" s="61"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="69"/>
+      <c r="P47" s="59"/>
+      <c r="Q47" s="59"/>
+      <c r="R47" s="59"/>
       <c r="S47">
         <v>45</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4487,29 +4524,29 @@
       <c r="F48" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G48" s="57" t="s">
+      <c r="G48" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H48" s="58"/>
-      <c r="I48" s="59"/>
-      <c r="J48" s="62" t="s">
+      <c r="H48" s="61"/>
+      <c r="I48" s="62"/>
+      <c r="J48" s="58" t="s">
         <v>200</v>
       </c>
-      <c r="K48" s="62"/>
-      <c r="L48" s="62"/>
-      <c r="M48" s="82" t="s">
+      <c r="K48" s="58"/>
+      <c r="L48" s="58"/>
+      <c r="M48" s="69" t="s">
         <v>201</v>
       </c>
-      <c r="N48" s="82"/>
-      <c r="O48" s="82"/>
-      <c r="P48" s="61"/>
-      <c r="Q48" s="61"/>
-      <c r="R48" s="61"/>
+      <c r="N48" s="69"/>
+      <c r="O48" s="69"/>
+      <c r="P48" s="59"/>
+      <c r="Q48" s="59"/>
+      <c r="R48" s="59"/>
       <c r="S48" s="28">
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:19">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4528,29 +4565,29 @@
       <c r="F49" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G49" s="57" t="s">
+      <c r="G49" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H49" s="58"/>
-      <c r="I49" s="59"/>
-      <c r="J49" s="62" t="s">
+      <c r="H49" s="61"/>
+      <c r="I49" s="62"/>
+      <c r="J49" s="58" t="s">
         <v>204</v>
       </c>
-      <c r="K49" s="62"/>
-      <c r="L49" s="62"/>
-      <c r="M49" s="82" t="s">
+      <c r="K49" s="58"/>
+      <c r="L49" s="58"/>
+      <c r="M49" s="69" t="s">
         <v>205</v>
       </c>
-      <c r="N49" s="82"/>
-      <c r="O49" s="82"/>
-      <c r="P49" s="61"/>
-      <c r="Q49" s="61"/>
-      <c r="R49" s="61"/>
+      <c r="N49" s="69"/>
+      <c r="O49" s="69"/>
+      <c r="P49" s="59"/>
+      <c r="Q49" s="59"/>
+      <c r="R49" s="59"/>
       <c r="S49">
         <v>47</v>
       </c>
     </row>
-    <row r="50" spans="1:19">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="30">
         <v>48</v>
       </c>
@@ -4569,29 +4606,29 @@
       <c r="F50" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G50" s="57" t="s">
+      <c r="G50" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H50" s="58"/>
-      <c r="I50" s="59"/>
-      <c r="J50" s="62" t="s">
+      <c r="H50" s="61"/>
+      <c r="I50" s="62"/>
+      <c r="J50" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="K50" s="62"/>
-      <c r="L50" s="62"/>
-      <c r="M50" s="82" t="s">
+      <c r="K50" s="58"/>
+      <c r="L50" s="58"/>
+      <c r="M50" s="69" t="s">
         <v>209</v>
       </c>
-      <c r="N50" s="82"/>
-      <c r="O50" s="82"/>
-      <c r="P50" s="61"/>
-      <c r="Q50" s="61"/>
-      <c r="R50" s="61"/>
+      <c r="N50" s="69"/>
+      <c r="O50" s="69"/>
+      <c r="P50" s="59"/>
+      <c r="Q50" s="59"/>
+      <c r="R50" s="59"/>
       <c r="S50" s="28">
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:19">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4610,64 +4647,64 @@
       <c r="F51" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G51" s="57" t="s">
+      <c r="G51" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="58"/>
-      <c r="I51" s="59"/>
-      <c r="J51" s="62" t="s">
+      <c r="H51" s="61"/>
+      <c r="I51" s="62"/>
+      <c r="J51" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="K51" s="62"/>
-      <c r="L51" s="62"/>
-      <c r="M51" s="82" t="s">
+      <c r="K51" s="58"/>
+      <c r="L51" s="58"/>
+      <c r="M51" s="69" t="s">
         <v>213</v>
       </c>
-      <c r="N51" s="82"/>
-      <c r="O51" s="82"/>
-      <c r="P51" s="61"/>
-      <c r="Q51" s="61"/>
-      <c r="R51" s="61"/>
+      <c r="N51" s="69"/>
+      <c r="O51" s="69"/>
+      <c r="P51" s="59"/>
+      <c r="Q51" s="59"/>
+      <c r="R51" s="59"/>
       <c r="S51">
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="1:19">
-      <c r="P52" s="61"/>
-      <c r="Q52" s="61"/>
-      <c r="R52" s="61"/>
-    </row>
-    <row r="53" spans="1:19">
-      <c r="P53" s="61"/>
-      <c r="Q53" s="61"/>
-      <c r="R53" s="61"/>
-    </row>
-    <row r="54" spans="1:19">
-      <c r="P54" s="61"/>
-      <c r="Q54" s="61"/>
-      <c r="R54" s="61"/>
-    </row>
-    <row r="55" spans="1:19">
-      <c r="P55" s="61"/>
-      <c r="Q55" s="61"/>
-      <c r="R55" s="61"/>
-    </row>
-    <row r="56" spans="1:19">
-      <c r="P56" s="61"/>
-      <c r="Q56" s="61"/>
-      <c r="R56" s="61"/>
-    </row>
-    <row r="57" spans="1:19">
-      <c r="P57" s="61"/>
-      <c r="Q57" s="61"/>
-      <c r="R57" s="61"/>
-    </row>
-    <row r="58" spans="1:19">
-      <c r="P58" s="61"/>
-      <c r="Q58" s="61"/>
-      <c r="R58" s="61"/>
-    </row>
-    <row r="59" spans="1:19">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P52" s="59"/>
+      <c r="Q52" s="59"/>
+      <c r="R52" s="59"/>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P53" s="59"/>
+      <c r="Q53" s="59"/>
+      <c r="R53" s="59"/>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P54" s="59"/>
+      <c r="Q54" s="59"/>
+      <c r="R54" s="59"/>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P55" s="59"/>
+      <c r="Q55" s="59"/>
+      <c r="R55" s="59"/>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P56" s="59"/>
+      <c r="Q56" s="59"/>
+      <c r="R56" s="59"/>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P57" s="59"/>
+      <c r="Q57" s="59"/>
+      <c r="R57" s="59"/>
+    </row>
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="P58" s="59"/>
+      <c r="Q58" s="59"/>
+      <c r="R58" s="59"/>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>214</v>
       </c>
@@ -4679,7 +4716,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="60" spans="1:19">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B60" s="10"/>
       <c r="C60" t="s">
         <v>215</v>
@@ -4688,7 +4725,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="61" spans="1:19">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B61" s="21"/>
       <c r="C61" t="s">
         <v>215</v>
@@ -4697,7 +4734,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="62" spans="1:19">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B62" s="29"/>
       <c r="C62" s="28" t="s">
         <v>219</v>
@@ -4706,7 +4743,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="79" spans="2:15">
+    <row r="79" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B79" s="9"/>
       <c r="C79" s="12"/>
       <c r="D79" s="11"/>
@@ -4715,14 +4752,14 @@
       <c r="G79" s="11"/>
       <c r="H79" s="11"/>
       <c r="I79" s="27"/>
-      <c r="J79" s="62"/>
-      <c r="K79" s="62"/>
-      <c r="L79" s="62"/>
-      <c r="M79" s="61"/>
-      <c r="N79" s="61"/>
-      <c r="O79" s="61"/>
-    </row>
-    <row r="80" spans="2:15">
+      <c r="J79" s="58"/>
+      <c r="K79" s="58"/>
+      <c r="L79" s="58"/>
+      <c r="M79" s="59"/>
+      <c r="N79" s="59"/>
+      <c r="O79" s="59"/>
+    </row>
+    <row r="80" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B80" s="9"/>
       <c r="C80" s="12"/>
       <c r="D80" s="11"/>
@@ -4731,14 +4768,14 @@
       <c r="G80" s="11"/>
       <c r="H80" s="11"/>
       <c r="I80" s="27"/>
-      <c r="J80" s="107"/>
-      <c r="K80" s="107"/>
-      <c r="L80" s="107"/>
-      <c r="M80" s="61"/>
-      <c r="N80" s="61"/>
-      <c r="O80" s="61"/>
-    </row>
-    <row r="81" spans="2:15">
+      <c r="J80" s="64"/>
+      <c r="K80" s="64"/>
+      <c r="L80" s="64"/>
+      <c r="M80" s="59"/>
+      <c r="N80" s="59"/>
+      <c r="O80" s="59"/>
+    </row>
+    <row r="81" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B81" s="9"/>
       <c r="C81" s="14"/>
       <c r="D81" s="11"/>
@@ -4747,14 +4784,14 @@
       <c r="G81" s="11"/>
       <c r="H81" s="11"/>
       <c r="I81" s="11"/>
-      <c r="J81" s="60"/>
-      <c r="K81" s="60"/>
-      <c r="L81" s="60"/>
-      <c r="M81" s="61"/>
-      <c r="N81" s="61"/>
-      <c r="O81" s="61"/>
-    </row>
-    <row r="82" spans="2:15">
+      <c r="J81" s="63"/>
+      <c r="K81" s="63"/>
+      <c r="L81" s="63"/>
+      <c r="M81" s="59"/>
+      <c r="N81" s="59"/>
+      <c r="O81" s="59"/>
+    </row>
+    <row r="82" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B82" s="9"/>
       <c r="C82" s="12"/>
       <c r="D82" s="11"/>
@@ -4763,14 +4800,14 @@
       <c r="G82" s="11"/>
       <c r="H82" s="11"/>
       <c r="I82" s="11"/>
-      <c r="J82" s="107"/>
-      <c r="K82" s="107"/>
-      <c r="L82" s="107"/>
-      <c r="M82" s="65"/>
-      <c r="N82" s="65"/>
-      <c r="O82" s="65"/>
-    </row>
-    <row r="83" spans="2:15">
+      <c r="J82" s="64"/>
+      <c r="K82" s="64"/>
+      <c r="L82" s="64"/>
+      <c r="M82" s="67"/>
+      <c r="N82" s="67"/>
+      <c r="O82" s="67"/>
+    </row>
+    <row r="83" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B83" s="9"/>
       <c r="C83" s="12"/>
       <c r="D83" s="11"/>
@@ -4779,14 +4816,14 @@
       <c r="G83" s="11"/>
       <c r="H83" s="11"/>
       <c r="I83" s="11"/>
-      <c r="J83" s="107"/>
-      <c r="K83" s="107"/>
-      <c r="L83" s="107"/>
-      <c r="M83" s="61"/>
-      <c r="N83" s="61"/>
-      <c r="O83" s="61"/>
-    </row>
-    <row r="84" spans="2:15">
+      <c r="J83" s="64"/>
+      <c r="K83" s="64"/>
+      <c r="L83" s="64"/>
+      <c r="M83" s="59"/>
+      <c r="N83" s="59"/>
+      <c r="O83" s="59"/>
+    </row>
+    <row r="84" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B84" s="9"/>
       <c r="C84" s="12"/>
       <c r="D84" s="11"/>
@@ -4795,14 +4832,14 @@
       <c r="G84" s="11"/>
       <c r="H84" s="11"/>
       <c r="I84" s="11"/>
-      <c r="J84" s="107"/>
-      <c r="K84" s="107"/>
-      <c r="L84" s="107"/>
-      <c r="M84" s="61"/>
-      <c r="N84" s="61"/>
-      <c r="O84" s="61"/>
-    </row>
-    <row r="85" spans="2:15">
+      <c r="J84" s="64"/>
+      <c r="K84" s="64"/>
+      <c r="L84" s="64"/>
+      <c r="M84" s="59"/>
+      <c r="N84" s="59"/>
+      <c r="O84" s="59"/>
+    </row>
+    <row r="85" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B85" s="9"/>
       <c r="C85" s="12"/>
       <c r="D85" s="11"/>
@@ -4811,14 +4848,14 @@
       <c r="G85" s="11"/>
       <c r="H85" s="11"/>
       <c r="I85" s="11"/>
-      <c r="J85" s="60"/>
-      <c r="K85" s="60"/>
-      <c r="L85" s="60"/>
-      <c r="M85" s="61"/>
-      <c r="N85" s="61"/>
-      <c r="O85" s="61"/>
-    </row>
-    <row r="86" spans="2:15">
+      <c r="J85" s="63"/>
+      <c r="K85" s="63"/>
+      <c r="L85" s="63"/>
+      <c r="M85" s="59"/>
+      <c r="N85" s="59"/>
+      <c r="O85" s="59"/>
+    </row>
+    <row r="86" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B86" s="9"/>
       <c r="C86" s="12"/>
       <c r="D86" s="11"/>
@@ -4827,14 +4864,14 @@
       <c r="G86" s="11"/>
       <c r="H86" s="11"/>
       <c r="I86" s="11"/>
-      <c r="J86" s="107"/>
-      <c r="K86" s="107"/>
-      <c r="L86" s="107"/>
-      <c r="M86" s="61"/>
-      <c r="N86" s="61"/>
-      <c r="O86" s="61"/>
-    </row>
-    <row r="87" spans="2:15">
+      <c r="J86" s="64"/>
+      <c r="K86" s="64"/>
+      <c r="L86" s="64"/>
+      <c r="M86" s="59"/>
+      <c r="N86" s="59"/>
+      <c r="O86" s="59"/>
+    </row>
+    <row r="87" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B87" s="9"/>
       <c r="C87" s="12"/>
       <c r="D87" s="11"/>
@@ -4843,14 +4880,14 @@
       <c r="G87" s="11"/>
       <c r="H87" s="11"/>
       <c r="I87" s="11"/>
-      <c r="J87" s="60"/>
-      <c r="K87" s="60"/>
-      <c r="L87" s="60"/>
-      <c r="M87" s="61"/>
-      <c r="N87" s="61"/>
-      <c r="O87" s="61"/>
-    </row>
-    <row r="88" spans="2:15">
+      <c r="J87" s="63"/>
+      <c r="K87" s="63"/>
+      <c r="L87" s="63"/>
+      <c r="M87" s="59"/>
+      <c r="N87" s="59"/>
+      <c r="O87" s="59"/>
+    </row>
+    <row r="88" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B88" s="9"/>
       <c r="C88" s="12"/>
       <c r="D88" s="11"/>
@@ -4859,14 +4896,14 @@
       <c r="G88" s="11"/>
       <c r="H88" s="11"/>
       <c r="I88" s="11"/>
-      <c r="J88" s="60"/>
-      <c r="K88" s="60"/>
-      <c r="L88" s="60"/>
-      <c r="M88" s="61"/>
-      <c r="N88" s="61"/>
-      <c r="O88" s="61"/>
-    </row>
-    <row r="89" spans="2:15">
+      <c r="J88" s="63"/>
+      <c r="K88" s="63"/>
+      <c r="L88" s="63"/>
+      <c r="M88" s="59"/>
+      <c r="N88" s="59"/>
+      <c r="O88" s="59"/>
+    </row>
+    <row r="89" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B89" s="9"/>
       <c r="C89" s="12"/>
       <c r="D89" s="11"/>
@@ -4875,14 +4912,14 @@
       <c r="G89" s="11"/>
       <c r="H89" s="11"/>
       <c r="I89" s="11"/>
-      <c r="J89" s="63"/>
-      <c r="K89" s="63"/>
-      <c r="L89" s="63"/>
-      <c r="M89" s="61"/>
-      <c r="N89" s="61"/>
-      <c r="O89" s="61"/>
-    </row>
-    <row r="90" spans="2:15">
+      <c r="J89" s="68"/>
+      <c r="K89" s="68"/>
+      <c r="L89" s="68"/>
+      <c r="M89" s="59"/>
+      <c r="N89" s="59"/>
+      <c r="O89" s="59"/>
+    </row>
+    <row r="90" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B90" s="9"/>
       <c r="C90" s="12"/>
       <c r="D90" s="11"/>
@@ -4891,14 +4928,14 @@
       <c r="G90" s="11"/>
       <c r="H90" s="11"/>
       <c r="I90" s="11"/>
-      <c r="J90" s="64"/>
-      <c r="K90" s="64"/>
-      <c r="L90" s="64"/>
-      <c r="M90" s="61"/>
-      <c r="N90" s="61"/>
-      <c r="O90" s="61"/>
-    </row>
-    <row r="91" spans="2:15">
+      <c r="J90" s="65"/>
+      <c r="K90" s="65"/>
+      <c r="L90" s="65"/>
+      <c r="M90" s="59"/>
+      <c r="N90" s="59"/>
+      <c r="O90" s="59"/>
+    </row>
+    <row r="91" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B91" s="9"/>
       <c r="C91" s="12"/>
       <c r="D91" s="11"/>
@@ -4907,14 +4944,14 @@
       <c r="G91" s="11"/>
       <c r="H91" s="11"/>
       <c r="I91" s="11"/>
-      <c r="J91" s="62"/>
-      <c r="K91" s="62"/>
-      <c r="L91" s="62"/>
-      <c r="M91" s="65"/>
-      <c r="N91" s="65"/>
-      <c r="O91" s="65"/>
-    </row>
-    <row r="92" spans="2:15">
+      <c r="J91" s="58"/>
+      <c r="K91" s="58"/>
+      <c r="L91" s="58"/>
+      <c r="M91" s="67"/>
+      <c r="N91" s="67"/>
+      <c r="O91" s="67"/>
+    </row>
+    <row r="92" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B92" s="9"/>
       <c r="C92" s="12"/>
       <c r="D92" s="11"/>
@@ -4923,14 +4960,14 @@
       <c r="G92" s="11"/>
       <c r="H92" s="11"/>
       <c r="I92" s="11"/>
-      <c r="J92" s="64"/>
-      <c r="K92" s="64"/>
-      <c r="L92" s="64"/>
-      <c r="M92" s="61"/>
-      <c r="N92" s="61"/>
-      <c r="O92" s="61"/>
-    </row>
-    <row r="93" spans="2:15">
+      <c r="J92" s="65"/>
+      <c r="K92" s="65"/>
+      <c r="L92" s="65"/>
+      <c r="M92" s="59"/>
+      <c r="N92" s="59"/>
+      <c r="O92" s="59"/>
+    </row>
+    <row r="93" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B93" s="9"/>
       <c r="C93" s="12"/>
       <c r="D93" s="11"/>
@@ -4939,14 +4976,14 @@
       <c r="G93" s="11"/>
       <c r="H93" s="11"/>
       <c r="I93" s="11"/>
-      <c r="J93" s="64"/>
-      <c r="K93" s="64"/>
-      <c r="L93" s="64"/>
-      <c r="M93" s="61"/>
-      <c r="N93" s="61"/>
-      <c r="O93" s="61"/>
-    </row>
-    <row r="94" spans="2:15">
+      <c r="J93" s="65"/>
+      <c r="K93" s="65"/>
+      <c r="L93" s="65"/>
+      <c r="M93" s="59"/>
+      <c r="N93" s="59"/>
+      <c r="O93" s="59"/>
+    </row>
+    <row r="94" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B94" s="9"/>
       <c r="C94" s="12"/>
       <c r="D94" s="11"/>
@@ -4955,512 +4992,287 @@
       <c r="G94" s="11"/>
       <c r="H94" s="11"/>
       <c r="I94" s="11"/>
-      <c r="J94" s="64"/>
-      <c r="K94" s="64"/>
-      <c r="L94" s="64"/>
-      <c r="M94" s="61"/>
-      <c r="N94" s="61"/>
-      <c r="O94" s="61"/>
-    </row>
-    <row r="95" spans="2:15">
+      <c r="J94" s="65"/>
+      <c r="K94" s="65"/>
+      <c r="L94" s="65"/>
+      <c r="M94" s="59"/>
+      <c r="N94" s="59"/>
+      <c r="O94" s="59"/>
+    </row>
+    <row r="95" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B95" s="9"/>
       <c r="C95" s="15"/>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
       <c r="F95" s="11"/>
-      <c r="G95" s="57"/>
-      <c r="H95" s="58"/>
-      <c r="I95" s="59"/>
-      <c r="J95" s="60"/>
-      <c r="K95" s="60"/>
-      <c r="L95" s="60"/>
-      <c r="M95" s="61"/>
-      <c r="N95" s="61"/>
-      <c r="O95" s="61"/>
-    </row>
-    <row r="96" spans="2:15">
+      <c r="G95" s="60"/>
+      <c r="H95" s="61"/>
+      <c r="I95" s="62"/>
+      <c r="J95" s="63"/>
+      <c r="K95" s="63"/>
+      <c r="L95" s="63"/>
+      <c r="M95" s="59"/>
+      <c r="N95" s="59"/>
+      <c r="O95" s="59"/>
+    </row>
+    <row r="96" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B96" s="9"/>
       <c r="C96" s="10"/>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
       <c r="F96" s="11"/>
-      <c r="G96" s="57"/>
-      <c r="H96" s="58"/>
-      <c r="I96" s="59"/>
-      <c r="J96" s="108"/>
-      <c r="K96" s="108"/>
-      <c r="L96" s="108"/>
-      <c r="M96" s="61"/>
-      <c r="N96" s="61"/>
-      <c r="O96" s="61"/>
-    </row>
-    <row r="97" spans="2:15">
+      <c r="G96" s="60"/>
+      <c r="H96" s="61"/>
+      <c r="I96" s="62"/>
+      <c r="J96" s="66"/>
+      <c r="K96" s="66"/>
+      <c r="L96" s="66"/>
+      <c r="M96" s="59"/>
+      <c r="N96" s="59"/>
+      <c r="O96" s="59"/>
+    </row>
+    <row r="97" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B97" s="9"/>
       <c r="C97" s="10"/>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
       <c r="F97" s="11"/>
-      <c r="G97" s="57"/>
-      <c r="H97" s="58"/>
-      <c r="I97" s="59"/>
-      <c r="J97" s="107"/>
-      <c r="K97" s="107"/>
-      <c r="L97" s="107"/>
-      <c r="M97" s="61"/>
-      <c r="N97" s="61"/>
-      <c r="O97" s="61"/>
-    </row>
-    <row r="98" spans="2:15">
+      <c r="G97" s="60"/>
+      <c r="H97" s="61"/>
+      <c r="I97" s="62"/>
+      <c r="J97" s="64"/>
+      <c r="K97" s="64"/>
+      <c r="L97" s="64"/>
+      <c r="M97" s="59"/>
+      <c r="N97" s="59"/>
+      <c r="O97" s="59"/>
+    </row>
+    <row r="98" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B98" s="9"/>
       <c r="C98" s="10"/>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
       <c r="F98" s="11"/>
-      <c r="G98" s="57"/>
-      <c r="H98" s="58"/>
-      <c r="I98" s="59"/>
-      <c r="J98" s="107"/>
-      <c r="K98" s="107"/>
-      <c r="L98" s="107"/>
-      <c r="M98" s="61"/>
-      <c r="N98" s="61"/>
-      <c r="O98" s="61"/>
-    </row>
-    <row r="99" spans="2:15">
+      <c r="G98" s="60"/>
+      <c r="H98" s="61"/>
+      <c r="I98" s="62"/>
+      <c r="J98" s="64"/>
+      <c r="K98" s="64"/>
+      <c r="L98" s="64"/>
+      <c r="M98" s="59"/>
+      <c r="N98" s="59"/>
+      <c r="O98" s="59"/>
+    </row>
+    <row r="99" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B99" s="9"/>
       <c r="C99" s="10"/>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
       <c r="F99" s="11"/>
-      <c r="G99" s="57"/>
-      <c r="H99" s="58"/>
-      <c r="I99" s="59"/>
-      <c r="J99" s="60"/>
-      <c r="K99" s="60"/>
-      <c r="L99" s="60"/>
-      <c r="M99" s="61"/>
-      <c r="N99" s="61"/>
-      <c r="O99" s="61"/>
-    </row>
-    <row r="100" spans="2:15">
+      <c r="G99" s="60"/>
+      <c r="H99" s="61"/>
+      <c r="I99" s="62"/>
+      <c r="J99" s="63"/>
+      <c r="K99" s="63"/>
+      <c r="L99" s="63"/>
+      <c r="M99" s="59"/>
+      <c r="N99" s="59"/>
+      <c r="O99" s="59"/>
+    </row>
+    <row r="100" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B100" s="9"/>
       <c r="C100" s="10"/>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
       <c r="F100" s="11"/>
-      <c r="G100" s="57"/>
-      <c r="H100" s="58"/>
-      <c r="I100" s="59"/>
-      <c r="J100" s="60"/>
-      <c r="K100" s="60"/>
-      <c r="L100" s="60"/>
-      <c r="M100" s="61"/>
-      <c r="N100" s="61"/>
-      <c r="O100" s="61"/>
-    </row>
-    <row r="101" spans="2:15">
+      <c r="G100" s="60"/>
+      <c r="H100" s="61"/>
+      <c r="I100" s="62"/>
+      <c r="J100" s="63"/>
+      <c r="K100" s="63"/>
+      <c r="L100" s="63"/>
+      <c r="M100" s="59"/>
+      <c r="N100" s="59"/>
+      <c r="O100" s="59"/>
+    </row>
+    <row r="101" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B101" s="9"/>
       <c r="C101" s="10"/>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
       <c r="F101" s="11"/>
-      <c r="G101" s="57"/>
-      <c r="H101" s="58"/>
-      <c r="I101" s="59"/>
-      <c r="J101" s="60"/>
-      <c r="K101" s="60"/>
-      <c r="L101" s="60"/>
-      <c r="M101" s="61"/>
-      <c r="N101" s="61"/>
-      <c r="O101" s="61"/>
-    </row>
-    <row r="102" spans="2:15">
+      <c r="G101" s="60"/>
+      <c r="H101" s="61"/>
+      <c r="I101" s="62"/>
+      <c r="J101" s="63"/>
+      <c r="K101" s="63"/>
+      <c r="L101" s="63"/>
+      <c r="M101" s="59"/>
+      <c r="N101" s="59"/>
+      <c r="O101" s="59"/>
+    </row>
+    <row r="102" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B102" s="9"/>
       <c r="C102" s="10"/>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
       <c r="F102" s="11"/>
-      <c r="G102" s="57"/>
-      <c r="H102" s="58"/>
-      <c r="I102" s="59"/>
-      <c r="J102" s="62"/>
-      <c r="K102" s="62"/>
-      <c r="L102" s="62"/>
-      <c r="M102" s="61"/>
-      <c r="N102" s="61"/>
-      <c r="O102" s="61"/>
-    </row>
-    <row r="103" spans="2:15">
+      <c r="G102" s="60"/>
+      <c r="H102" s="61"/>
+      <c r="I102" s="62"/>
+      <c r="J102" s="58"/>
+      <c r="K102" s="58"/>
+      <c r="L102" s="58"/>
+      <c r="M102" s="59"/>
+      <c r="N102" s="59"/>
+      <c r="O102" s="59"/>
+    </row>
+    <row r="103" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B103" s="9"/>
       <c r="C103" s="10"/>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
       <c r="F103" s="11"/>
-      <c r="G103" s="57"/>
-      <c r="H103" s="58"/>
-      <c r="I103" s="59"/>
-      <c r="J103" s="62"/>
-      <c r="K103" s="62"/>
-      <c r="L103" s="62"/>
-      <c r="M103" s="61"/>
-      <c r="N103" s="61"/>
-      <c r="O103" s="61"/>
-    </row>
-    <row r="104" spans="2:15">
+      <c r="G103" s="60"/>
+      <c r="H103" s="61"/>
+      <c r="I103" s="62"/>
+      <c r="J103" s="58"/>
+      <c r="K103" s="58"/>
+      <c r="L103" s="58"/>
+      <c r="M103" s="59"/>
+      <c r="N103" s="59"/>
+      <c r="O103" s="59"/>
+    </row>
+    <row r="104" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B104" s="9"/>
       <c r="C104" s="10"/>
       <c r="D104" s="11"/>
       <c r="E104" s="11"/>
       <c r="F104" s="11"/>
-      <c r="G104" s="57"/>
-      <c r="H104" s="58"/>
-      <c r="I104" s="59"/>
-      <c r="J104" s="60"/>
-      <c r="K104" s="60"/>
-      <c r="L104" s="60"/>
-      <c r="M104" s="61"/>
-      <c r="N104" s="61"/>
-      <c r="O104" s="61"/>
-    </row>
-    <row r="105" spans="2:15">
+      <c r="G104" s="60"/>
+      <c r="H104" s="61"/>
+      <c r="I104" s="62"/>
+      <c r="J104" s="63"/>
+      <c r="K104" s="63"/>
+      <c r="L104" s="63"/>
+      <c r="M104" s="59"/>
+      <c r="N104" s="59"/>
+      <c r="O104" s="59"/>
+    </row>
+    <row r="105" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B105" s="9"/>
       <c r="C105" s="10"/>
       <c r="D105" s="11"/>
       <c r="E105" s="11"/>
       <c r="F105" s="11"/>
-      <c r="G105" s="57"/>
-      <c r="H105" s="58"/>
-      <c r="I105" s="59"/>
-      <c r="J105" s="62"/>
-      <c r="K105" s="62"/>
-      <c r="L105" s="62"/>
-      <c r="M105" s="61"/>
-      <c r="N105" s="61"/>
-      <c r="O105" s="61"/>
-    </row>
-    <row r="106" spans="2:15">
+      <c r="G105" s="60"/>
+      <c r="H105" s="61"/>
+      <c r="I105" s="62"/>
+      <c r="J105" s="58"/>
+      <c r="K105" s="58"/>
+      <c r="L105" s="58"/>
+      <c r="M105" s="59"/>
+      <c r="N105" s="59"/>
+      <c r="O105" s="59"/>
+    </row>
+    <row r="106" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B106" s="9"/>
       <c r="C106" s="10"/>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
       <c r="F106" s="11"/>
-      <c r="G106" s="57"/>
-      <c r="H106" s="58"/>
-      <c r="I106" s="59"/>
-      <c r="J106" s="62"/>
-      <c r="K106" s="62"/>
-      <c r="L106" s="62"/>
-      <c r="M106" s="61"/>
-      <c r="N106" s="61"/>
-      <c r="O106" s="61"/>
-    </row>
-    <row r="107" spans="2:15">
+      <c r="G106" s="60"/>
+      <c r="H106" s="61"/>
+      <c r="I106" s="62"/>
+      <c r="J106" s="58"/>
+      <c r="K106" s="58"/>
+      <c r="L106" s="58"/>
+      <c r="M106" s="59"/>
+      <c r="N106" s="59"/>
+      <c r="O106" s="59"/>
+    </row>
+    <row r="107" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B107" s="19"/>
       <c r="C107" s="10"/>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
       <c r="F107" s="11"/>
-      <c r="G107" s="57"/>
-      <c r="H107" s="58"/>
-      <c r="I107" s="59"/>
-      <c r="J107" s="62"/>
-      <c r="K107" s="62"/>
-      <c r="L107" s="62"/>
-      <c r="M107" s="61"/>
-      <c r="N107" s="61"/>
-      <c r="O107" s="61"/>
-    </row>
-    <row r="108" spans="2:15">
+      <c r="G107" s="60"/>
+      <c r="H107" s="61"/>
+      <c r="I107" s="62"/>
+      <c r="J107" s="58"/>
+      <c r="K107" s="58"/>
+      <c r="L107" s="58"/>
+      <c r="M107" s="59"/>
+      <c r="N107" s="59"/>
+      <c r="O107" s="59"/>
+    </row>
+    <row r="108" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B108" s="19"/>
       <c r="C108" s="10"/>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
       <c r="F108" s="11"/>
-      <c r="G108" s="57"/>
-      <c r="H108" s="58"/>
-      <c r="I108" s="59"/>
-      <c r="J108" s="62"/>
-      <c r="K108" s="62"/>
-      <c r="L108" s="62"/>
-      <c r="M108" s="61"/>
-      <c r="N108" s="61"/>
-      <c r="O108" s="61"/>
-    </row>
-    <row r="109" spans="2:15">
+      <c r="G108" s="60"/>
+      <c r="H108" s="61"/>
+      <c r="I108" s="62"/>
+      <c r="J108" s="58"/>
+      <c r="K108" s="58"/>
+      <c r="L108" s="58"/>
+      <c r="M108" s="59"/>
+      <c r="N108" s="59"/>
+      <c r="O108" s="59"/>
+    </row>
+    <row r="109" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B109" s="19"/>
       <c r="C109" s="10"/>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
       <c r="F109" s="11"/>
-      <c r="G109" s="57"/>
-      <c r="H109" s="58"/>
-      <c r="I109" s="59"/>
-      <c r="J109" s="62"/>
-      <c r="K109" s="62"/>
-      <c r="L109" s="62"/>
-      <c r="M109" s="61"/>
-      <c r="N109" s="61"/>
-      <c r="O109" s="61"/>
-    </row>
-    <row r="110" spans="2:15">
+      <c r="G109" s="60"/>
+      <c r="H109" s="61"/>
+      <c r="I109" s="62"/>
+      <c r="J109" s="58"/>
+      <c r="K109" s="58"/>
+      <c r="L109" s="58"/>
+      <c r="M109" s="59"/>
+      <c r="N109" s="59"/>
+      <c r="O109" s="59"/>
+    </row>
+    <row r="110" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B110" s="19"/>
       <c r="C110" s="10"/>
       <c r="D110" s="11"/>
       <c r="E110" s="11"/>
       <c r="F110" s="11"/>
-      <c r="G110" s="57"/>
-      <c r="H110" s="58"/>
-      <c r="I110" s="59"/>
-      <c r="J110" s="62"/>
-      <c r="K110" s="62"/>
-      <c r="L110" s="62"/>
-      <c r="M110" s="61"/>
-      <c r="N110" s="61"/>
-      <c r="O110" s="61"/>
-    </row>
-    <row r="111" spans="2:15">
+      <c r="G110" s="60"/>
+      <c r="H110" s="61"/>
+      <c r="I110" s="62"/>
+      <c r="J110" s="58"/>
+      <c r="K110" s="58"/>
+      <c r="L110" s="58"/>
+      <c r="M110" s="59"/>
+      <c r="N110" s="59"/>
+      <c r="O110" s="59"/>
+    </row>
+    <row r="111" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B111" s="9"/>
       <c r="C111" s="16"/>
       <c r="D111" s="11"/>
-      <c r="E111" s="76"/>
-      <c r="F111" s="77"/>
-      <c r="G111" s="77"/>
-      <c r="H111" s="77"/>
-      <c r="I111" s="78"/>
-      <c r="J111" s="62"/>
-      <c r="K111" s="62"/>
-      <c r="L111" s="62"/>
-      <c r="M111" s="61"/>
-      <c r="N111" s="61"/>
-      <c r="O111" s="61"/>
+      <c r="E111" s="55"/>
+      <c r="F111" s="56"/>
+      <c r="G111" s="56"/>
+      <c r="H111" s="56"/>
+      <c r="I111" s="57"/>
+      <c r="J111" s="58"/>
+      <c r="K111" s="58"/>
+      <c r="L111" s="58"/>
+      <c r="M111" s="59"/>
+      <c r="N111" s="59"/>
+      <c r="O111" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="243">
-    <mergeCell ref="E111:I111"/>
-    <mergeCell ref="J111:L111"/>
-    <mergeCell ref="M111:O111"/>
-    <mergeCell ref="G109:I109"/>
-    <mergeCell ref="J109:L109"/>
-    <mergeCell ref="M109:O109"/>
-    <mergeCell ref="G110:I110"/>
-    <mergeCell ref="J110:L110"/>
-    <mergeCell ref="M110:O110"/>
-    <mergeCell ref="G107:I107"/>
-    <mergeCell ref="J107:L107"/>
-    <mergeCell ref="M107:O107"/>
-    <mergeCell ref="G108:I108"/>
-    <mergeCell ref="J108:L108"/>
-    <mergeCell ref="M108:O108"/>
-    <mergeCell ref="G105:I105"/>
-    <mergeCell ref="J105:L105"/>
-    <mergeCell ref="M105:O105"/>
-    <mergeCell ref="G106:I106"/>
-    <mergeCell ref="J106:L106"/>
-    <mergeCell ref="M106:O106"/>
-    <mergeCell ref="G103:I103"/>
-    <mergeCell ref="J103:L103"/>
-    <mergeCell ref="M103:O103"/>
-    <mergeCell ref="G104:I104"/>
-    <mergeCell ref="J104:L104"/>
-    <mergeCell ref="M104:O104"/>
-    <mergeCell ref="G101:I101"/>
-    <mergeCell ref="J101:L101"/>
-    <mergeCell ref="M101:O101"/>
-    <mergeCell ref="G102:I102"/>
-    <mergeCell ref="J102:L102"/>
-    <mergeCell ref="M102:O102"/>
-    <mergeCell ref="G99:I99"/>
-    <mergeCell ref="J99:L99"/>
-    <mergeCell ref="M99:O99"/>
-    <mergeCell ref="G100:I100"/>
-    <mergeCell ref="J100:L100"/>
-    <mergeCell ref="M100:O100"/>
-    <mergeCell ref="G97:I97"/>
-    <mergeCell ref="J97:L97"/>
-    <mergeCell ref="M97:O97"/>
-    <mergeCell ref="G98:I98"/>
-    <mergeCell ref="J98:L98"/>
-    <mergeCell ref="M98:O98"/>
-    <mergeCell ref="J94:L94"/>
-    <mergeCell ref="M94:O94"/>
-    <mergeCell ref="G95:I95"/>
-    <mergeCell ref="J95:L95"/>
-    <mergeCell ref="M95:O95"/>
-    <mergeCell ref="G96:I96"/>
-    <mergeCell ref="J96:L96"/>
-    <mergeCell ref="M96:O96"/>
-    <mergeCell ref="J91:L91"/>
-    <mergeCell ref="M91:O91"/>
-    <mergeCell ref="J92:L92"/>
-    <mergeCell ref="M92:O92"/>
-    <mergeCell ref="J93:L93"/>
-    <mergeCell ref="M93:O93"/>
-    <mergeCell ref="J88:L88"/>
-    <mergeCell ref="M88:O88"/>
-    <mergeCell ref="J89:L89"/>
-    <mergeCell ref="M89:O89"/>
-    <mergeCell ref="J90:L90"/>
-    <mergeCell ref="M90:O90"/>
-    <mergeCell ref="J85:L85"/>
-    <mergeCell ref="M85:O85"/>
-    <mergeCell ref="J86:L86"/>
-    <mergeCell ref="M86:O86"/>
-    <mergeCell ref="J87:L87"/>
-    <mergeCell ref="M87:O87"/>
-    <mergeCell ref="J82:L82"/>
-    <mergeCell ref="M82:O82"/>
-    <mergeCell ref="J83:L83"/>
-    <mergeCell ref="M83:O83"/>
-    <mergeCell ref="J84:L84"/>
-    <mergeCell ref="M84:O84"/>
-    <mergeCell ref="P58:R58"/>
-    <mergeCell ref="J79:L79"/>
-    <mergeCell ref="M79:O79"/>
-    <mergeCell ref="J80:L80"/>
-    <mergeCell ref="M80:O80"/>
-    <mergeCell ref="J81:L81"/>
-    <mergeCell ref="M81:O81"/>
-    <mergeCell ref="P52:R52"/>
-    <mergeCell ref="P53:R53"/>
-    <mergeCell ref="P54:R54"/>
-    <mergeCell ref="P55:R55"/>
-    <mergeCell ref="P56:R56"/>
-    <mergeCell ref="P57:R57"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="M50:O50"/>
-    <mergeCell ref="P50:R50"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="M51:O51"/>
-    <mergeCell ref="P51:R51"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="M48:O48"/>
-    <mergeCell ref="P48:R48"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="M49:O49"/>
-    <mergeCell ref="P49:R49"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="M46:O46"/>
-    <mergeCell ref="P46:R46"/>
-    <mergeCell ref="G47:I47"/>
-    <mergeCell ref="J47:L47"/>
-    <mergeCell ref="M47:O47"/>
-    <mergeCell ref="P47:R47"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="M44:O44"/>
-    <mergeCell ref="P44:R44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="M45:O45"/>
-    <mergeCell ref="P45:R45"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="M42:O42"/>
-    <mergeCell ref="P42:R42"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="J43:L43"/>
-    <mergeCell ref="M43:O43"/>
-    <mergeCell ref="P43:R43"/>
-    <mergeCell ref="G40:I40"/>
-    <mergeCell ref="J40:L40"/>
-    <mergeCell ref="M40:O40"/>
-    <mergeCell ref="P40:R40"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="P41:R41"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="M38:O38"/>
-    <mergeCell ref="P38:R38"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="M39:O39"/>
-    <mergeCell ref="P39:R39"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="M36:O36"/>
-    <mergeCell ref="P36:R36"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:L37"/>
-    <mergeCell ref="M37:O37"/>
-    <mergeCell ref="P37:R37"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="M34:O34"/>
-    <mergeCell ref="P34:R34"/>
-    <mergeCell ref="J35:L35"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="P35:R35"/>
-    <mergeCell ref="E32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="M32:O32"/>
-    <mergeCell ref="P32:R32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="J33:L33"/>
-    <mergeCell ref="M33:O33"/>
-    <mergeCell ref="P33:R33"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="P30:R30"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:L31"/>
-    <mergeCell ref="M31:O31"/>
-    <mergeCell ref="P31:R31"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:L28"/>
-    <mergeCell ref="M28:O28"/>
-    <mergeCell ref="P28:R28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="M29:O29"/>
-    <mergeCell ref="P29:R29"/>
-    <mergeCell ref="J26:L26"/>
-    <mergeCell ref="M26:O26"/>
-    <mergeCell ref="P26:R26"/>
-    <mergeCell ref="J27:L27"/>
-    <mergeCell ref="M27:O27"/>
-    <mergeCell ref="P27:R27"/>
-    <mergeCell ref="J23:L23"/>
-    <mergeCell ref="M23:O23"/>
-    <mergeCell ref="J24:L24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="M25:O25"/>
-    <mergeCell ref="J20:L20"/>
-    <mergeCell ref="M20:O20"/>
-    <mergeCell ref="P20:R20"/>
-    <mergeCell ref="J21:L21"/>
-    <mergeCell ref="M21:O21"/>
-    <mergeCell ref="J22:L22"/>
-    <mergeCell ref="M22:O22"/>
-    <mergeCell ref="J17:L17"/>
-    <mergeCell ref="M17:O17"/>
-    <mergeCell ref="J18:L18"/>
-    <mergeCell ref="M18:O18"/>
-    <mergeCell ref="J19:L19"/>
-    <mergeCell ref="M19:O19"/>
-    <mergeCell ref="J14:L14"/>
-    <mergeCell ref="M14:O14"/>
-    <mergeCell ref="J15:L15"/>
-    <mergeCell ref="M15:O15"/>
-    <mergeCell ref="J16:L16"/>
-    <mergeCell ref="M16:O16"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="M12:O12"/>
-    <mergeCell ref="J13:L13"/>
-    <mergeCell ref="M13:O13"/>
-    <mergeCell ref="J8:L8"/>
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="J9:L9"/>
-    <mergeCell ref="M9:O9"/>
     <mergeCell ref="J1:L1"/>
     <mergeCell ref="M2:O2"/>
     <mergeCell ref="G3:I3"/>
@@ -5479,6 +5291,231 @@
     <mergeCell ref="M6:O6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="M7:O7"/>
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="J13:L13"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="J9:L9"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="J17:L17"/>
+    <mergeCell ref="M17:O17"/>
+    <mergeCell ref="J18:L18"/>
+    <mergeCell ref="M18:O18"/>
+    <mergeCell ref="J19:L19"/>
+    <mergeCell ref="M19:O19"/>
+    <mergeCell ref="J14:L14"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="J15:L15"/>
+    <mergeCell ref="M15:O15"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="M23:O23"/>
+    <mergeCell ref="J24:L24"/>
+    <mergeCell ref="M24:O24"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="M25:O25"/>
+    <mergeCell ref="J20:L20"/>
+    <mergeCell ref="M20:O20"/>
+    <mergeCell ref="P20:R20"/>
+    <mergeCell ref="J21:L21"/>
+    <mergeCell ref="M21:O21"/>
+    <mergeCell ref="J22:L22"/>
+    <mergeCell ref="M22:O22"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:L28"/>
+    <mergeCell ref="M28:O28"/>
+    <mergeCell ref="P28:R28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="M29:O29"/>
+    <mergeCell ref="P29:R29"/>
+    <mergeCell ref="J26:L26"/>
+    <mergeCell ref="M26:O26"/>
+    <mergeCell ref="P26:R26"/>
+    <mergeCell ref="J27:L27"/>
+    <mergeCell ref="M27:O27"/>
+    <mergeCell ref="P27:R27"/>
+    <mergeCell ref="E32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="M32:O32"/>
+    <mergeCell ref="P32:R32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="J33:L33"/>
+    <mergeCell ref="M33:O33"/>
+    <mergeCell ref="P33:R33"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="P30:R30"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:L31"/>
+    <mergeCell ref="M31:O31"/>
+    <mergeCell ref="P31:R31"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="M36:O36"/>
+    <mergeCell ref="P36:R36"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:L37"/>
+    <mergeCell ref="M37:O37"/>
+    <mergeCell ref="P37:R37"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="M34:O34"/>
+    <mergeCell ref="P34:R34"/>
+    <mergeCell ref="J35:L35"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="P35:R35"/>
+    <mergeCell ref="G40:I40"/>
+    <mergeCell ref="J40:L40"/>
+    <mergeCell ref="M40:O40"/>
+    <mergeCell ref="P40:R40"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="P41:R41"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="M38:O38"/>
+    <mergeCell ref="P38:R38"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="M39:O39"/>
+    <mergeCell ref="P39:R39"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="M44:O44"/>
+    <mergeCell ref="P44:R44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="M45:O45"/>
+    <mergeCell ref="P45:R45"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="M42:O42"/>
+    <mergeCell ref="P42:R42"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="J43:L43"/>
+    <mergeCell ref="M43:O43"/>
+    <mergeCell ref="P43:R43"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="M48:O48"/>
+    <mergeCell ref="P48:R48"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="M49:O49"/>
+    <mergeCell ref="P49:R49"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="M46:O46"/>
+    <mergeCell ref="P46:R46"/>
+    <mergeCell ref="G47:I47"/>
+    <mergeCell ref="J47:L47"/>
+    <mergeCell ref="M47:O47"/>
+    <mergeCell ref="P47:R47"/>
+    <mergeCell ref="P52:R52"/>
+    <mergeCell ref="P53:R53"/>
+    <mergeCell ref="P54:R54"/>
+    <mergeCell ref="P55:R55"/>
+    <mergeCell ref="P56:R56"/>
+    <mergeCell ref="P57:R57"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="M50:O50"/>
+    <mergeCell ref="P50:R50"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="M51:O51"/>
+    <mergeCell ref="P51:R51"/>
+    <mergeCell ref="J82:L82"/>
+    <mergeCell ref="M82:O82"/>
+    <mergeCell ref="J83:L83"/>
+    <mergeCell ref="M83:O83"/>
+    <mergeCell ref="J84:L84"/>
+    <mergeCell ref="M84:O84"/>
+    <mergeCell ref="P58:R58"/>
+    <mergeCell ref="J79:L79"/>
+    <mergeCell ref="M79:O79"/>
+    <mergeCell ref="J80:L80"/>
+    <mergeCell ref="M80:O80"/>
+    <mergeCell ref="J81:L81"/>
+    <mergeCell ref="M81:O81"/>
+    <mergeCell ref="J88:L88"/>
+    <mergeCell ref="M88:O88"/>
+    <mergeCell ref="J89:L89"/>
+    <mergeCell ref="M89:O89"/>
+    <mergeCell ref="J90:L90"/>
+    <mergeCell ref="M90:O90"/>
+    <mergeCell ref="J85:L85"/>
+    <mergeCell ref="M85:O85"/>
+    <mergeCell ref="J86:L86"/>
+    <mergeCell ref="M86:O86"/>
+    <mergeCell ref="J87:L87"/>
+    <mergeCell ref="M87:O87"/>
+    <mergeCell ref="J94:L94"/>
+    <mergeCell ref="M94:O94"/>
+    <mergeCell ref="G95:I95"/>
+    <mergeCell ref="J95:L95"/>
+    <mergeCell ref="M95:O95"/>
+    <mergeCell ref="G96:I96"/>
+    <mergeCell ref="J96:L96"/>
+    <mergeCell ref="M96:O96"/>
+    <mergeCell ref="J91:L91"/>
+    <mergeCell ref="M91:O91"/>
+    <mergeCell ref="J92:L92"/>
+    <mergeCell ref="M92:O92"/>
+    <mergeCell ref="J93:L93"/>
+    <mergeCell ref="M93:O93"/>
+    <mergeCell ref="G99:I99"/>
+    <mergeCell ref="J99:L99"/>
+    <mergeCell ref="M99:O99"/>
+    <mergeCell ref="G100:I100"/>
+    <mergeCell ref="J100:L100"/>
+    <mergeCell ref="M100:O100"/>
+    <mergeCell ref="G97:I97"/>
+    <mergeCell ref="J97:L97"/>
+    <mergeCell ref="M97:O97"/>
+    <mergeCell ref="G98:I98"/>
+    <mergeCell ref="J98:L98"/>
+    <mergeCell ref="M98:O98"/>
+    <mergeCell ref="G103:I103"/>
+    <mergeCell ref="J103:L103"/>
+    <mergeCell ref="M103:O103"/>
+    <mergeCell ref="G104:I104"/>
+    <mergeCell ref="J104:L104"/>
+    <mergeCell ref="M104:O104"/>
+    <mergeCell ref="G101:I101"/>
+    <mergeCell ref="J101:L101"/>
+    <mergeCell ref="M101:O101"/>
+    <mergeCell ref="G102:I102"/>
+    <mergeCell ref="J102:L102"/>
+    <mergeCell ref="M102:O102"/>
+    <mergeCell ref="G107:I107"/>
+    <mergeCell ref="J107:L107"/>
+    <mergeCell ref="M107:O107"/>
+    <mergeCell ref="G108:I108"/>
+    <mergeCell ref="J108:L108"/>
+    <mergeCell ref="M108:O108"/>
+    <mergeCell ref="G105:I105"/>
+    <mergeCell ref="J105:L105"/>
+    <mergeCell ref="M105:O105"/>
+    <mergeCell ref="G106:I106"/>
+    <mergeCell ref="J106:L106"/>
+    <mergeCell ref="M106:O106"/>
+    <mergeCell ref="E111:I111"/>
+    <mergeCell ref="J111:L111"/>
+    <mergeCell ref="M111:O111"/>
+    <mergeCell ref="G109:I109"/>
+    <mergeCell ref="J109:L109"/>
+    <mergeCell ref="M109:O109"/>
+    <mergeCell ref="G110:I110"/>
+    <mergeCell ref="J110:L110"/>
+    <mergeCell ref="M110:O110"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
@@ -5491,31 +5528,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D43" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="H50" sqref="H50"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D47" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="7" width="13.125" style="38" customWidth="1"/>
-    <col min="8" max="8" width="50.25" style="38" customWidth="1"/>
-    <col min="9" max="9" width="13.125" style="38" customWidth="1"/>
-    <col min="10" max="10" width="15.125" style="38" customWidth="1"/>
-    <col min="11" max="11" width="14.875" style="38" customWidth="1"/>
-    <col min="12" max="12" width="13.125" style="38" customWidth="1"/>
+    <col min="3" max="3" width="16.59765625" customWidth="1"/>
+    <col min="4" max="7" width="13.09765625" style="38" customWidth="1"/>
+    <col min="8" max="8" width="50.19921875" style="38" customWidth="1"/>
+    <col min="9" max="9" width="13.09765625" style="38" customWidth="1"/>
+    <col min="10" max="10" width="15.09765625" style="38" customWidth="1"/>
+    <col min="11" max="11" width="14.8984375" style="38" customWidth="1"/>
+    <col min="12" max="12" width="13.09765625" style="38" customWidth="1"/>
     <col min="13" max="13" width="15.5" style="38" customWidth="1"/>
-    <col min="14" max="14" width="17.375" style="38" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" style="38" customWidth="1"/>
     <col min="15" max="15" width="17" style="38" customWidth="1"/>
-    <col min="16" max="16" width="31.375" style="38" customWidth="1"/>
-    <col min="17" max="19" width="13.125" style="38" customWidth="1"/>
-    <col min="20" max="21" width="13.125" customWidth="1"/>
+    <col min="16" max="16" width="31.3984375" style="38" customWidth="1"/>
+    <col min="17" max="19" width="13.09765625" style="38" customWidth="1"/>
+    <col min="20" max="21" width="13.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="56.25" customHeight="1">
+    <row r="1" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C1" s="44" t="s">
         <v>221</v>
       </c>
@@ -5568,7 +5605,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="46" customFormat="1" ht="56.25" customHeight="1">
+    <row r="2" spans="1:19" s="46" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="47"/>
       <c r="B2" s="47"/>
       <c r="C2" s="49" t="s">
@@ -5621,7 +5658,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="56.25" customHeight="1">
+    <row r="3" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="39">
         <v>1</v>
       </c>
@@ -5670,7 +5707,7 @@
       <c r="R3"/>
       <c r="S3"/>
     </row>
-    <row r="4" spans="1:19" ht="56.25" customHeight="1">
+    <row r="4" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="41">
         <v>2</v>
       </c>
@@ -5719,7 +5756,7 @@
       <c r="R4"/>
       <c r="S4"/>
     </row>
-    <row r="5" spans="1:19" ht="56.25" customHeight="1">
+    <row r="5" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39">
         <v>3</v>
       </c>
@@ -5768,7 +5805,7 @@
       <c r="R5" s="53"/>
       <c r="S5" s="53"/>
     </row>
-    <row r="6" spans="1:19" ht="56.25" customHeight="1">
+    <row r="6" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="42">
         <v>4</v>
       </c>
@@ -5817,7 +5854,7 @@
       <c r="R6" s="53"/>
       <c r="S6" s="53"/>
     </row>
-    <row r="7" spans="1:19" ht="56.25" customHeight="1">
+    <row r="7" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="41">
         <v>5</v>
       </c>
@@ -5866,7 +5903,7 @@
       <c r="R7" s="53"/>
       <c r="S7" s="53"/>
     </row>
-    <row r="8" spans="1:19" ht="56.25" customHeight="1">
+    <row r="8" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="39">
         <v>6</v>
       </c>
@@ -5915,7 +5952,7 @@
       <c r="R8" s="53"/>
       <c r="S8" s="53"/>
     </row>
-    <row r="9" spans="1:19" ht="56.25" customHeight="1">
+    <row r="9" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="39">
         <v>7</v>
       </c>
@@ -5964,7 +6001,7 @@
       <c r="R9" s="53"/>
       <c r="S9" s="53"/>
     </row>
-    <row r="10" spans="1:19" ht="56.25" customHeight="1">
+    <row r="10" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="39">
         <v>8</v>
       </c>
@@ -5978,13 +6015,13 @@
         <v>254</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F10" s="53" t="s">
         <v>255</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>20</v>
+        <v>255</v>
       </c>
       <c r="H10" s="53" t="s">
         <v>269</v>
@@ -6013,7 +6050,7 @@
       <c r="R10" s="53"/>
       <c r="S10" s="53"/>
     </row>
-    <row r="11" spans="1:19" ht="56.25" customHeight="1">
+    <row r="11" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="39">
         <v>9</v>
       </c>
@@ -6062,7 +6099,7 @@
       <c r="R11" s="53"/>
       <c r="S11" s="53"/>
     </row>
-    <row r="12" spans="1:19" ht="56.25" customHeight="1">
+    <row r="12" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="41">
         <v>10</v>
       </c>
@@ -6111,7 +6148,7 @@
       <c r="R12" s="53"/>
       <c r="S12" s="53"/>
     </row>
-    <row r="13" spans="1:19" ht="56.25" customHeight="1">
+    <row r="13" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="39">
         <v>11</v>
       </c>
@@ -6160,7 +6197,7 @@
       <c r="R13" s="53"/>
       <c r="S13" s="53"/>
     </row>
-    <row r="14" spans="1:19" ht="56.25" customHeight="1">
+    <row r="14" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="42">
         <v>12</v>
       </c>
@@ -6209,7 +6246,7 @@
       <c r="R14" s="53"/>
       <c r="S14" s="53"/>
     </row>
-    <row r="15" spans="1:19" ht="56.25" customHeight="1">
+    <row r="15" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="41">
         <v>13</v>
       </c>
@@ -6258,7 +6295,7 @@
       <c r="R15" s="53"/>
       <c r="S15" s="53"/>
     </row>
-    <row r="16" spans="1:19" ht="56.25" customHeight="1">
+    <row r="16" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="41">
         <v>14</v>
       </c>
@@ -6307,7 +6344,7 @@
       <c r="R16" s="53"/>
       <c r="S16" s="53"/>
     </row>
-    <row r="17" spans="1:19" ht="56.25" customHeight="1">
+    <row r="17" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="41">
         <v>15</v>
       </c>
@@ -6356,7 +6393,7 @@
       <c r="R17" s="53"/>
       <c r="S17" s="53"/>
     </row>
-    <row r="18" spans="1:19" ht="56.25" customHeight="1">
+    <row r="18" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="41">
         <v>16</v>
       </c>
@@ -6405,7 +6442,7 @@
       <c r="R18" s="53"/>
       <c r="S18" s="53"/>
     </row>
-    <row r="19" spans="1:19" ht="56.25" customHeight="1">
+    <row r="19" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="41">
         <v>17</v>
       </c>
@@ -6454,26 +6491,26 @@
       <c r="R19" s="53"/>
       <c r="S19" s="53"/>
     </row>
-    <row r="20" spans="1:19" ht="31.5" customHeight="1">
-      <c r="A20" s="96">
+    <row r="20" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="105">
         <v>18</v>
       </c>
-      <c r="B20" s="98" t="s">
+      <c r="B20" s="101" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="100" t="s">
+      <c r="C20" s="103" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="102" t="s">
+      <c r="D20" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="E20" s="102" t="s">
+      <c r="E20" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="F20" s="102" t="s">
+      <c r="F20" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="G20" s="102" t="s">
+      <c r="G20" s="97" t="s">
         <v>20</v>
       </c>
       <c r="H20" s="53" t="s">
@@ -6503,14 +6540,14 @@
       <c r="R20" s="53"/>
       <c r="S20" s="53"/>
     </row>
-    <row r="21" spans="1:19" ht="31.5" customHeight="1">
-      <c r="A21" s="97"/>
-      <c r="B21" s="99"/>
-      <c r="C21" s="101"/>
-      <c r="D21" s="103"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="103"/>
-      <c r="G21" s="103"/>
+    <row r="21" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="106"/>
+      <c r="B21" s="102"/>
+      <c r="C21" s="104"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
       <c r="H21" s="53" t="s">
         <v>279</v>
       </c>
@@ -6536,26 +6573,26 @@
       <c r="R21" s="53"/>
       <c r="S21" s="53"/>
     </row>
-    <row r="22" spans="1:19" ht="31.5" customHeight="1">
-      <c r="A22" s="104">
+    <row r="22" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="99">
         <v>19</v>
       </c>
-      <c r="B22" s="98" t="s">
+      <c r="B22" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="100" t="s">
+      <c r="C22" s="103" t="s">
         <v>103</v>
       </c>
-      <c r="D22" s="102" t="s">
+      <c r="D22" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="E22" s="102" t="s">
+      <c r="E22" s="97" t="s">
         <v>253</v>
       </c>
-      <c r="F22" s="102" t="s">
+      <c r="F22" s="97" t="s">
         <v>19</v>
       </c>
-      <c r="G22" s="102" t="s">
+      <c r="G22" s="97" t="s">
         <v>20</v>
       </c>
       <c r="H22" s="53" t="s">
@@ -6585,14 +6622,14 @@
       <c r="R22" s="53"/>
       <c r="S22" s="53"/>
     </row>
-    <row r="23" spans="1:19" ht="31.5" customHeight="1">
-      <c r="A23" s="105"/>
-      <c r="B23" s="99"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
+    <row r="23" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="100"/>
+      <c r="B23" s="102"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98"/>
       <c r="H23" s="53" t="s">
         <v>281</v>
       </c>
@@ -6618,7 +6655,7 @@
       <c r="R23" s="53"/>
       <c r="S23" s="53"/>
     </row>
-    <row r="24" spans="1:19" ht="56.25" customHeight="1">
+    <row r="24" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39">
         <v>20</v>
       </c>
@@ -6667,7 +6704,7 @@
       <c r="R24" s="53"/>
       <c r="S24" s="53"/>
     </row>
-    <row r="25" spans="1:19" ht="56.25" customHeight="1">
+    <row r="25" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="39">
         <v>21</v>
       </c>
@@ -6716,7 +6753,7 @@
       <c r="R25" s="53"/>
       <c r="S25" s="53"/>
     </row>
-    <row r="26" spans="1:19" ht="56.25" customHeight="1">
+    <row r="26" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="39">
         <v>22</v>
       </c>
@@ -6765,7 +6802,7 @@
       <c r="R26" s="53"/>
       <c r="S26" s="53"/>
     </row>
-    <row r="27" spans="1:19" ht="56.25" customHeight="1">
+    <row r="27" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="39">
         <v>23</v>
       </c>
@@ -6814,7 +6851,7 @@
       <c r="R27" s="53"/>
       <c r="S27" s="53"/>
     </row>
-    <row r="28" spans="1:19" ht="56.25" customHeight="1">
+    <row r="28" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39">
         <v>24</v>
       </c>
@@ -6863,7 +6900,7 @@
       <c r="R28" s="53"/>
       <c r="S28" s="53"/>
     </row>
-    <row r="29" spans="1:19" ht="56.25" customHeight="1">
+    <row r="29" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39">
         <v>25</v>
       </c>
@@ -6912,7 +6949,7 @@
       <c r="R29" s="53"/>
       <c r="S29" s="53"/>
     </row>
-    <row r="30" spans="1:19" ht="56.25" customHeight="1">
+    <row r="30" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39">
         <v>26</v>
       </c>
@@ -6961,7 +6998,7 @@
       <c r="R30" s="53"/>
       <c r="S30" s="53"/>
     </row>
-    <row r="31" spans="1:19" ht="56.25" customHeight="1">
+    <row r="31" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="39">
         <v>27</v>
       </c>
@@ -7010,7 +7047,7 @@
       <c r="R31" s="53"/>
       <c r="S31" s="53"/>
     </row>
-    <row r="32" spans="1:19" ht="56.25" customHeight="1">
+    <row r="32" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="42">
         <v>28</v>
       </c>
@@ -7059,7 +7096,7 @@
       <c r="R32" s="53"/>
       <c r="S32" s="53"/>
     </row>
-    <row r="33" spans="1:19" ht="56.25" customHeight="1">
+    <row r="33" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="41">
         <v>29</v>
       </c>
@@ -7082,14 +7119,14 @@
         <v>255</v>
       </c>
       <c r="H33" s="53" t="s">
-        <v>288</v>
+        <v>323</v>
       </c>
       <c r="I33" s="53"/>
       <c r="J33" s="53" t="s">
         <v>257</v>
       </c>
       <c r="K33" s="53" t="s">
-        <v>258</v>
+        <v>322</v>
       </c>
       <c r="L33" s="53" t="s">
         <v>20</v>
@@ -7108,7 +7145,7 @@
       <c r="R33" s="53"/>
       <c r="S33" s="53"/>
     </row>
-    <row r="34" spans="1:19" ht="56.25" customHeight="1">
+    <row r="34" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="39">
         <v>30</v>
       </c>
@@ -7157,7 +7194,7 @@
       <c r="R34" s="53"/>
       <c r="S34" s="53"/>
     </row>
-    <row r="35" spans="1:19" ht="56.25" customHeight="1">
+    <row r="35" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="39">
         <v>31</v>
       </c>
@@ -7184,7 +7221,7 @@
       </c>
       <c r="I35" s="53"/>
       <c r="J35" s="53" t="s">
-        <v>270</v>
+        <v>324</v>
       </c>
       <c r="K35" s="53" t="s">
         <v>270</v>
@@ -7206,7 +7243,7 @@
       <c r="R35" s="53"/>
       <c r="S35" s="53"/>
     </row>
-    <row r="36" spans="1:19" ht="56.25" customHeight="1">
+    <row r="36" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="39">
         <v>32</v>
       </c>
@@ -7255,7 +7292,7 @@
       <c r="R36" s="53"/>
       <c r="S36" s="53"/>
     </row>
-    <row r="37" spans="1:19" ht="56.25" customHeight="1">
+    <row r="37" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="41">
         <v>33</v>
       </c>
@@ -7304,7 +7341,7 @@
       <c r="R37" s="53"/>
       <c r="S37" s="53"/>
     </row>
-    <row r="38" spans="1:19" ht="56.25" customHeight="1">
+    <row r="38" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="39">
         <v>34</v>
       </c>
@@ -7353,7 +7390,7 @@
       <c r="R38" s="53"/>
       <c r="S38" s="53"/>
     </row>
-    <row r="39" spans="1:19" ht="56.25" customHeight="1">
+    <row r="39" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="41">
         <v>35</v>
       </c>
@@ -7402,7 +7439,7 @@
       <c r="R39" s="53"/>
       <c r="S39" s="53"/>
     </row>
-    <row r="40" spans="1:19" ht="56.25" customHeight="1">
+    <row r="40" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="42">
         <v>36</v>
       </c>
@@ -7451,7 +7488,7 @@
       <c r="R40" s="53"/>
       <c r="S40" s="53"/>
     </row>
-    <row r="41" spans="1:19" ht="56.25" customHeight="1">
+    <row r="41" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="41">
         <v>37</v>
       </c>
@@ -7500,7 +7537,7 @@
       <c r="R41" s="53"/>
       <c r="S41" s="53"/>
     </row>
-    <row r="42" spans="1:19" ht="56.25" customHeight="1">
+    <row r="42" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="39">
         <v>38</v>
       </c>
@@ -7549,7 +7586,7 @@
       <c r="R42" s="53"/>
       <c r="S42" s="53"/>
     </row>
-    <row r="43" spans="1:19" ht="56.25" customHeight="1">
+    <row r="43" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="41">
         <v>39</v>
       </c>
@@ -7598,7 +7635,7 @@
       <c r="R43" s="53"/>
       <c r="S43" s="53"/>
     </row>
-    <row r="44" spans="1:19" ht="56.25" customHeight="1">
+    <row r="44" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="41">
         <v>40</v>
       </c>
@@ -7647,7 +7684,7 @@
       <c r="R44" s="53"/>
       <c r="S44" s="53"/>
     </row>
-    <row r="45" spans="1:19" ht="56.25" customHeight="1">
+    <row r="45" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="41">
         <v>41</v>
       </c>
@@ -7696,7 +7733,7 @@
       <c r="R45" s="53"/>
       <c r="S45" s="53"/>
     </row>
-    <row r="46" spans="1:19" ht="56.25" customHeight="1">
+    <row r="46" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="41">
         <v>42</v>
       </c>
@@ -7745,7 +7782,7 @@
       <c r="R46" s="53"/>
       <c r="S46" s="53"/>
     </row>
-    <row r="47" spans="1:19" ht="56.25" customHeight="1">
+    <row r="47" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="41">
         <v>43</v>
       </c>
@@ -7794,7 +7831,7 @@
       <c r="R47" s="53"/>
       <c r="S47" s="53"/>
     </row>
-    <row r="48" spans="1:19" ht="56.25" customHeight="1">
+    <row r="48" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="39">
         <v>44</v>
       </c>
@@ -7843,7 +7880,7 @@
       <c r="R48" s="53"/>
       <c r="S48" s="53"/>
     </row>
-    <row r="49" spans="1:19" ht="56.25" customHeight="1">
+    <row r="49" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="39">
         <v>45</v>
       </c>
@@ -7854,7 +7891,7 @@
         <v>195</v>
       </c>
       <c r="D49" s="53" t="s">
-        <v>254</v>
+        <v>325</v>
       </c>
       <c r="E49" s="53" t="s">
         <v>253</v>
@@ -7892,7 +7929,7 @@
       <c r="R49" s="53"/>
       <c r="S49" s="53"/>
     </row>
-    <row r="50" spans="1:19" ht="56.25" customHeight="1">
+    <row r="50" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="41">
         <v>46</v>
       </c>
@@ -7915,7 +7952,7 @@
         <v>255</v>
       </c>
       <c r="H50" s="53" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="I50" s="53"/>
       <c r="J50" s="53" t="s">
@@ -7941,7 +7978,7 @@
       <c r="R50" s="53"/>
       <c r="S50" s="53"/>
     </row>
-    <row r="51" spans="1:19" s="45" customFormat="1" ht="56.25" customHeight="1">
+    <row r="51" spans="1:19" s="45" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="41">
         <v>47</v>
       </c>
@@ -7952,7 +7989,7 @@
         <v>202</v>
       </c>
       <c r="D51" s="53" t="s">
-        <v>254</v>
+        <v>325</v>
       </c>
       <c r="E51" s="53" t="s">
         <v>253</v>
@@ -7964,7 +8001,7 @@
         <v>20</v>
       </c>
       <c r="H51" s="53" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I51" s="53"/>
       <c r="J51" s="53" t="s">
@@ -7990,7 +8027,7 @@
       <c r="R51" s="53"/>
       <c r="S51" s="53"/>
     </row>
-    <row r="52" spans="1:19" ht="56.25" customHeight="1">
+    <row r="52" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="42">
         <v>48</v>
       </c>
@@ -8013,7 +8050,7 @@
         <v>255</v>
       </c>
       <c r="H52" s="53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I52" s="53"/>
       <c r="J52" s="53" t="s">
@@ -8036,7 +8073,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="56.25" customHeight="1">
+    <row r="53" spans="1:19" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="41">
         <v>49</v>
       </c>
@@ -8047,7 +8084,7 @@
         <v>210</v>
       </c>
       <c r="D53" s="53" t="s">
-        <v>254</v>
+        <v>325</v>
       </c>
       <c r="E53" s="53" t="s">
         <v>253</v>
@@ -8059,7 +8096,7 @@
         <v>20</v>
       </c>
       <c r="H53" s="53" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I53" s="53"/>
       <c r="J53" s="53" t="s">
@@ -8084,6 +8121,13 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="B22:B23"/>
@@ -8091,17 +8135,10 @@
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="E22:E23"/>
     <mergeCell ref="F22:F23"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <headerFooter scaleWithDoc="0" alignWithMargins="0"/>
 </worksheet>
 </file>
@@ -8114,94 +8151,94 @@
       <selection activeCell="B1" sqref="B1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:3">
-      <c r="B1" s="80" t="s">
-        <v>321</v>
-      </c>
-      <c r="C1" s="81"/>
-    </row>
-    <row r="2" spans="2:3">
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-    </row>
-    <row r="3" spans="2:3">
-      <c r="B3" s="79" t="s">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="108" t="s">
+        <v>320</v>
+      </c>
+      <c r="C1" s="109"/>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="109"/>
+      <c r="C2" s="109"/>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="107" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="79"/>
-    </row>
-    <row r="4" spans="2:3">
-      <c r="B4" s="79" t="s">
+      <c r="C3" s="107"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="79"/>
-    </row>
-    <row r="5" spans="2:3">
+      <c r="C4" s="107"/>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="1"/>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1"/>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B9" s="1"/>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>
-    <row r="12" spans="2:3">
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="2:3">
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
     </row>
-    <row r="15" spans="2:3">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="2:2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="2:2">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" s="1"/>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" s="1"/>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish ex except little cute's part
</commit_message>
<xml_diff>
--- a/指令.xlsx
+++ b/指令.xlsx
@@ -1182,8 +1182,19 @@
     <t>rd = reg2_o&gt;&gt; reg1_o[4:0]</t>
   </si>
   <si>
-    <t>rd = reg2_o &gt;&gt; reg1_o[15:11]
-左侧补符号位</t>
+    <r>
+      <t xml:space="preserve">rd = reg2_o &gt;&gt; reg1_o[15:11]
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF4F4F4F"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>左侧补符号位</t>
+    </r>
   </si>
   <si>
     <t>rd = reg2_o &gt;&gt; reg1_o[4:0]
@@ -1390,12 +1401,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="47">
-    <font>
-      <sz val="12"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
+  <fonts count="46">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
@@ -1636,6 +1642,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF4F4F4F"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4F4F4F"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
@@ -1680,12 +1692,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FF333333"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <color indexed="63"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
@@ -1703,7 +1709,7 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1814,12 +1820,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1832,12 +1832,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1845,12 +1839,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2326,48 +2314,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="24" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -2377,97 +2368,94 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="19" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="19" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2475,7 +2463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2484,7 +2472,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
@@ -2493,34 +2481,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2529,31 +2517,31 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2562,97 +2550,97 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1">
@@ -2664,133 +2652,133 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="7" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="3" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -6097,11 +6085,11 @@
   <dimension ref="A1:S53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="D24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D33" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A29" sqref="$A29:$XFD29"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="$A37:$XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -7090,7 +7078,7 @@
         <v>255</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="L20" s="16" t="s">
         <v>37</v>
@@ -7172,7 +7160,7 @@
         <v>255</v>
       </c>
       <c r="K22" s="16" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="L22" s="16" t="s">
         <v>37</v>

</xml_diff>